<commit_message>
Update regions, GDP & Pop (Excel), sep. CI & EI
</commit_message>
<xml_diff>
--- a/model/inputdata/RICE_data.xlsx
+++ b/model/inputdata/RICE_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ef8a875e15b7533c/Bureaublad/Afstuderen/WRR/PyRICE Ivar Tjallingii/PyRICE2020/3_MOEA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maryamalki/Desktop/PyRICE_2022/model/inputdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{84B31132-8A08-43F2-A9C4-02788C84B45C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6430A47-A224-E545-B785-E850F9F0030D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{8CDEB586-1210-4D27-97A3-779EFE9372BB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23240" windowHeight="12560" xr2:uid="{8CDEB586-1210-4D27-97A3-779EFE9372BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -667,7 +667,7 @@
     <numFmt numFmtId="175" formatCode="#,##0.0000"/>
     <numFmt numFmtId="176" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1095,10 +1095,10 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Comma 2" xfId="3" xr:uid="{197BD7F7-F531-483E-A783-C0AA2B2C56E0}"/>
-    <cellStyle name="Komma" xfId="1" builtinId="3"/>
-    <cellStyle name="Procent" xfId="2" builtinId="5"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Per cent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -7604,7 +7604,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -7902,34 +7902,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2022DB91-C134-49BF-BD97-D84764B92169}">
   <dimension ref="A1:DR455"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="G99" sqref="G99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.3671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.7890625" customWidth="1"/>
-    <col min="2" max="2" width="10.15625" customWidth="1"/>
-    <col min="3" max="3" width="10.26171875" customWidth="1"/>
-    <col min="4" max="4" width="11.3671875" customWidth="1"/>
-    <col min="5" max="5" width="10.578125" customWidth="1"/>
-    <col min="6" max="6" width="11.1015625" customWidth="1"/>
-    <col min="7" max="7" width="11.5234375" customWidth="1"/>
-    <col min="8" max="8" width="10.83984375" customWidth="1"/>
-    <col min="9" max="9" width="10.578125" customWidth="1"/>
-    <col min="10" max="10" width="10.83984375" customWidth="1"/>
-    <col min="11" max="11" width="11.1015625" customWidth="1"/>
-    <col min="12" max="12" width="13.9453125" customWidth="1"/>
-    <col min="13" max="13" width="10.83984375" customWidth="1"/>
-    <col min="14" max="14" width="9.89453125" customWidth="1"/>
-    <col min="15" max="15" width="14.89453125" customWidth="1"/>
-    <col min="16" max="16" width="13.68359375" customWidth="1"/>
-    <col min="17" max="45" width="13.9453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="5" max="5" width="10.5" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" customWidth="1"/>
+    <col min="7" max="7" width="11.5" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" customWidth="1"/>
+    <col min="9" max="9" width="10.5" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" customWidth="1"/>
+    <col min="12" max="12" width="14" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" customWidth="1"/>
+    <col min="14" max="14" width="9.83203125" customWidth="1"/>
+    <col min="15" max="15" width="14.83203125" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" customWidth="1"/>
+    <col min="17" max="45" width="14" bestFit="1" customWidth="1"/>
     <col min="46" max="61" width="15" bestFit="1" customWidth="1"/>
-    <col min="122" max="122" width="8.7890625" bestFit="1" customWidth="1"/>
+    <col min="122" max="122" width="8.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:78">
+    <row r="1" spans="3:78" x14ac:dyDescent="0.2">
       <c r="F1" s="1">
         <f>+E4</f>
         <v>1.5093183403803685E-2</v>
@@ -7959,7 +7959,7 @@
         <v>1.2852478557080983E-2</v>
       </c>
     </row>
-    <row r="2" spans="3:78">
+    <row r="2" spans="3:78" x14ac:dyDescent="0.2">
       <c r="M2">
         <v>0</v>
       </c>
@@ -8208,7 +8208,7 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="3" spans="3:78" s="3" customFormat="1">
+    <row r="3" spans="3:78" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E3" s="3" t="s">
         <v>0</v>
       </c>
@@ -8473,7 +8473,7 @@
         <v>2595</v>
       </c>
     </row>
-    <row r="4" spans="3:78">
+    <row r="4" spans="3:78" x14ac:dyDescent="0.2">
       <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
@@ -8764,7 +8764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="3:78">
+    <row r="5" spans="3:78" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>9</v>
       </c>
@@ -9058,7 +9058,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="6" spans="3:78">
+    <row r="6" spans="3:78" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>10</v>
       </c>
@@ -9098,7 +9098,7 @@
         <v>34767.021932553827</v>
       </c>
       <c r="O6" s="6">
-        <f t="shared" ref="O6:AD16" si="18">+N6*(O$4/N$4)*(N$4*$J6/N6)^$K6</f>
+        <f t="shared" ref="O6:AD15" si="18">+N6*(O$4/N$4)*(N$4*$J6/N6)^$K6</f>
         <v>40905.99686077865</v>
       </c>
       <c r="P6" s="6">
@@ -9351,7 +9351,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="7" spans="3:78">
+    <row r="7" spans="3:78" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
         <v>11</v>
       </c>
@@ -9644,7 +9644,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="8" spans="3:78">
+    <row r="8" spans="3:78" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
         <v>12</v>
       </c>
@@ -9938,7 +9938,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="9" spans="3:78">
+    <row r="9" spans="3:78" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
         <v>13</v>
       </c>
@@ -10231,7 +10231,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="10" spans="3:78">
+    <row r="10" spans="3:78" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
         <v>14</v>
       </c>
@@ -10524,7 +10524,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="3:78">
+    <row r="11" spans="3:78" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
         <v>15</v>
       </c>
@@ -10817,7 +10817,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="3:78">
+    <row r="12" spans="3:78" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
         <v>16</v>
       </c>
@@ -11110,7 +11110,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="13" spans="3:78">
+    <row r="13" spans="3:78" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
         <v>17</v>
       </c>
@@ -11403,7 +11403,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="14" spans="3:78">
+    <row r="14" spans="3:78" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
         <v>18</v>
       </c>
@@ -11696,7 +11696,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="15" spans="3:78">
+    <row r="15" spans="3:78" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
         <v>19</v>
       </c>
@@ -11989,7 +11989,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="16" spans="3:78">
+    <row r="16" spans="3:78" x14ac:dyDescent="0.2">
       <c r="C16" s="9" t="s">
         <v>20</v>
       </c>
@@ -12243,7 +12243,7 @@
         <v>617571.06669911754</v>
       </c>
     </row>
-    <row r="17" spans="1:106">
+    <row r="17" spans="1:106" x14ac:dyDescent="0.2">
       <c r="J17" s="10">
         <f>+STDEV(J5:J15)</f>
         <v>0.17529196424044302</v>
@@ -12256,7 +12256,7 @@
       <c r="R17" s="12"/>
       <c r="S17" s="11"/>
     </row>
-    <row r="18" spans="1:106">
+    <row r="18" spans="1:106" x14ac:dyDescent="0.2">
       <c r="E18" t="s">
         <v>22</v>
       </c>
@@ -12264,12 +12264,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:106">
+    <row r="19" spans="1:106" x14ac:dyDescent="0.2">
       <c r="E19" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:106">
+    <row r="20" spans="1:106" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
         <v>25</v>
       </c>
@@ -12286,7 +12286,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:106">
+    <row r="21" spans="1:106" x14ac:dyDescent="0.2">
       <c r="A21" s="13">
         <f>+[2]sum_newregion!AF17/1000000</f>
         <v>296.842578</v>
@@ -12406,7 +12406,7 @@
       <c r="DA21" s="14"/>
       <c r="DB21" s="14"/>
     </row>
-    <row r="22" spans="1:106">
+    <row r="22" spans="1:106" x14ac:dyDescent="0.2">
       <c r="A22" s="13">
         <f>+[2]sum_newregion!AF18/1000000</f>
         <v>490.08019258719162</v>
@@ -12529,7 +12529,7 @@
       <c r="DA22" s="14"/>
       <c r="DB22" s="14"/>
     </row>
-    <row r="23" spans="1:106">
+    <row r="23" spans="1:106" x14ac:dyDescent="0.2">
       <c r="A23" s="13">
         <f>+[2]sum_newregion!AF19/1000000</f>
         <v>127.773</v>
@@ -12652,7 +12652,7 @@
       <c r="DA23" s="14"/>
       <c r="DB23" s="14"/>
     </row>
-    <row r="24" spans="1:106">
+    <row r="24" spans="1:106" x14ac:dyDescent="0.2">
       <c r="A24" s="13">
         <f>+[2]sum_newregion!AF20/1000000</f>
         <v>143.15</v>
@@ -12775,7 +12775,7 @@
       <c r="DA24" s="14"/>
       <c r="DB24" s="14"/>
     </row>
-    <row r="25" spans="1:106">
+    <row r="25" spans="1:106" x14ac:dyDescent="0.2">
       <c r="A25" s="13">
         <f>+[2]sum_newregion!AF21/1000000</f>
         <v>155.94246849385479</v>
@@ -12898,7 +12898,7 @@
       <c r="DA25" s="14"/>
       <c r="DB25" s="14"/>
     </row>
-    <row r="26" spans="1:106">
+    <row r="26" spans="1:106" x14ac:dyDescent="0.2">
       <c r="A26" s="13">
         <f>+[2]sum_newregion!AF22/1000000</f>
         <v>1304.5</v>
@@ -13020,7 +13020,7 @@
       <c r="DA26" s="14"/>
       <c r="DB26" s="14"/>
     </row>
-    <row r="27" spans="1:106">
+    <row r="27" spans="1:106" x14ac:dyDescent="0.2">
       <c r="A27" s="13">
         <f>+[2]sum_newregion!AF23/1000000</f>
         <v>1094.5830000000001</v>
@@ -13143,7 +13143,7 @@
       <c r="DA27" s="14"/>
       <c r="DB27" s="14"/>
     </row>
-    <row r="28" spans="1:106">
+    <row r="28" spans="1:106" x14ac:dyDescent="0.2">
       <c r="A28" s="13">
         <f>+[2]sum_newregion!AF24/1000000</f>
         <v>412.76900131562951</v>
@@ -13266,7 +13266,7 @@
       <c r="DA28" s="14"/>
       <c r="DB28" s="14"/>
     </row>
-    <row r="29" spans="1:106">
+    <row r="29" spans="1:106" x14ac:dyDescent="0.2">
       <c r="A29" s="13">
         <f>+[2]sum_newregion!AF25/1000000</f>
         <v>763.50611154103387</v>
@@ -13389,7 +13389,7 @@
       <c r="DA29" s="14"/>
       <c r="DB29" s="14"/>
     </row>
-    <row r="30" spans="1:106">
+    <row r="30" spans="1:106" x14ac:dyDescent="0.2">
       <c r="A30" s="13">
         <f>+[2]sum_newregion!AF26/1000000</f>
         <v>555.38007856447791</v>
@@ -13512,7 +13512,7 @@
       <c r="DA30" s="14"/>
       <c r="DB30" s="14"/>
     </row>
-    <row r="31" spans="1:106">
+    <row r="31" spans="1:106" x14ac:dyDescent="0.2">
       <c r="A31" s="13">
         <f>+[2]sum_newregion!AF27/1000000</f>
         <v>129.169624</v>
@@ -13635,7 +13635,7 @@
       <c r="DA31" s="14"/>
       <c r="DB31" s="14"/>
     </row>
-    <row r="32" spans="1:106">
+    <row r="32" spans="1:106" x14ac:dyDescent="0.2">
       <c r="A32" s="13">
         <f>+[2]sum_newregion!AF28/1000000</f>
         <v>937.19556697899202</v>
@@ -13758,7 +13758,7 @@
       <c r="DA32" s="14"/>
       <c r="DB32" s="14"/>
     </row>
-    <row r="33" spans="1:42">
+    <row r="33" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A33" s="13">
         <f>+[2]sum_newregion!AF29/1000000</f>
         <v>6418.8626225301014</v>
@@ -13799,7 +13799,7 @@
       <c r="AO33" s="14"/>
       <c r="AP33" s="14"/>
     </row>
-    <row r="34" spans="1:42">
+    <row r="34" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D34">
         <f>+LN([1]Parameters!B27)/20</f>
         <v>0</v>
@@ -13809,16 +13809,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:42" s="16" customFormat="1">
+    <row r="35" spans="1:42" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="15"/>
       <c r="AF35" s="17"/>
     </row>
-    <row r="36" spans="1:42" s="18" customFormat="1">
+    <row r="36" spans="1:42" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:42" s="18" customFormat="1">
+    <row r="37" spans="1:42" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="19" t="s">
         <v>31</v>
       </c>
@@ -13913,7 +13913,7 @@
         <v>2305</v>
       </c>
     </row>
-    <row r="38" spans="1:42" s="20" customFormat="1">
+    <row r="38" spans="1:42" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="20" t="s">
         <v>8</v>
       </c>
@@ -14029,7 +14029,7 @@
         <v>2.3885051393862582E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:42" s="20" customFormat="1">
+    <row r="39" spans="1:42" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="20" t="s">
         <v>9</v>
       </c>
@@ -14145,7 +14145,7 @@
         <v>3.1396723190096556E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:42" s="20" customFormat="1">
+    <row r="40" spans="1:42" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="20" t="s">
         <v>10</v>
       </c>
@@ -14261,7 +14261,7 @@
         <v>3.0840332648654197E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:42" s="20" customFormat="1">
+    <row r="41" spans="1:42" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="20" t="s">
         <v>11</v>
       </c>
@@ -14377,7 +14377,7 @@
         <v>2.7494542668942047E-4</v>
       </c>
     </row>
-    <row r="42" spans="1:42" s="20" customFormat="1">
+    <row r="42" spans="1:42" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="20" t="s">
         <v>12</v>
       </c>
@@ -14493,7 +14493,7 @@
         <v>2.6712831904026366E-4</v>
       </c>
     </row>
-    <row r="43" spans="1:42" s="20" customFormat="1">
+    <row r="43" spans="1:42" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="20" t="s">
         <v>13</v>
       </c>
@@ -14609,7 +14609,7 @@
         <v>3.400889125551121E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:42" s="20" customFormat="1">
+    <row r="44" spans="1:42" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>14</v>
       </c>
@@ -14725,7 +14725,7 @@
         <v>2.510562290461483E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:42" s="20" customFormat="1">
+    <row r="45" spans="1:42" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="20" t="s">
         <v>15</v>
       </c>
@@ -14841,7 +14841,7 @@
         <v>2.3184833799830409E-4</v>
       </c>
     </row>
-    <row r="46" spans="1:42" s="20" customFormat="1">
+    <row r="46" spans="1:42" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="20" t="s">
         <v>16</v>
       </c>
@@ -14957,7 +14957,7 @@
         <v>2.5369337346638232E-4</v>
       </c>
     </row>
-    <row r="47" spans="1:42" s="20" customFormat="1">
+    <row r="47" spans="1:42" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="20" t="s">
         <v>17</v>
       </c>
@@ -15073,7 +15073,7 @@
         <v>2.9863628279880783E-4</v>
       </c>
     </row>
-    <row r="48" spans="1:42" s="22" customFormat="1">
+    <row r="48" spans="1:42" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="20" t="s">
         <v>18</v>
       </c>
@@ -15184,7 +15184,7 @@
         <v>3.0167347725146889E-4</v>
       </c>
     </row>
-    <row r="49" spans="1:61" s="22" customFormat="1">
+    <row r="49" spans="1:61" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="20" t="s">
         <v>19</v>
       </c>
@@ -15295,7 +15295,7 @@
         <v>2.4588974617446705E-4</v>
       </c>
     </row>
-    <row r="53" spans="1:61" ht="17.399999999999999">
+    <row r="53" spans="1:61" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" s="23" t="s">
         <v>32</v>
       </c>
@@ -15393,7 +15393,7 @@
         <v>2305</v>
       </c>
     </row>
-    <row r="54" spans="1:61" s="2" customFormat="1">
+    <row r="54" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>8</v>
       </c>
@@ -15637,7 +15637,7 @@
         <v>2.3349931558640943E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:61" s="2" customFormat="1">
+    <row r="55" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>9</v>
       </c>
@@ -15881,7 +15881,7 @@
         <v>2.3407587288159313E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:61" s="2" customFormat="1">
+    <row r="56" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>10</v>
       </c>
@@ -16125,7 +16125,7 @@
         <v>2.3389443039658745E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:61" s="2" customFormat="1">
+    <row r="57" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>11</v>
       </c>
@@ -16369,7 +16369,7 @@
         <v>2.3460205621661226E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:61" s="2" customFormat="1">
+    <row r="58" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>12</v>
       </c>
@@ -16613,7 +16613,7 @@
         <v>2.3605473567992088E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:61" s="2" customFormat="1">
+    <row r="59" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>13</v>
       </c>
@@ -16857,7 +16857,7 @@
         <v>2.3565632618017746E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:61" s="2" customFormat="1">
+    <row r="60" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>14</v>
       </c>
@@ -17101,7 +17101,7 @@
         <v>2.3683465900772869E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:61" s="2" customFormat="1">
+    <row r="61" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>15</v>
       </c>
@@ -17345,7 +17345,7 @@
         <v>2.3491872836351353E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:61" s="2" customFormat="1">
+    <row r="62" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>16</v>
       </c>
@@ -17589,7 +17589,7 @@
         <v>2.3706992309963128E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:61" s="2" customFormat="1">
+    <row r="63" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>17</v>
       </c>
@@ -17833,7 +17833,7 @@
         <v>2.3544670821475065E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:61" s="2" customFormat="1">
+    <row r="64" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>18</v>
       </c>
@@ -18077,7 +18077,7 @@
         <v>2.3383882565285166E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:66" s="2" customFormat="1">
+    <row r="65" spans="1:66" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>19</v>
       </c>
@@ -18321,7 +18321,7 @@
         <v>2.3706248559144873E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:66">
+    <row r="66" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>33</v>
       </c>
@@ -18449,16 +18449,16 @@
         <v>3.0008485881581021E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:66">
+    <row r="68" spans="1:66" x14ac:dyDescent="0.2">
       <c r="H68" s="1"/>
     </row>
-    <row r="70" spans="1:66" ht="17.399999999999999">
+    <row r="70" spans="1:66" ht="18" x14ac:dyDescent="0.2">
       <c r="A70" s="23" t="s">
         <v>34</v>
       </c>
       <c r="B70" s="9"/>
     </row>
-    <row r="71" spans="1:66" ht="43.2">
+    <row r="71" spans="1:66" ht="48" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>35</v>
       </c>
@@ -18528,7 +18528,7 @@
         <v>2125</v>
       </c>
     </row>
-    <row r="72" spans="1:66">
+    <row r="72" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>8</v>
       </c>
@@ -18791,7 +18791,7 @@
         <v>-2.5332240062604858E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:66">
+    <row r="73" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A73" s="9" t="s">
         <v>41</v>
       </c>
@@ -18822,7 +18822,7 @@
         <v>-1.445723245068292E-2</v>
       </c>
       <c r="I73" s="29">
-        <f t="shared" ref="I73:X84" si="30">+$F73+(H73-$F73)*(1-$E73)</f>
+        <f t="shared" ref="I73:X83" si="30">+$F73+(H73-$F73)*(1-$E73)</f>
         <v>-1.3261509205614629E-2</v>
       </c>
       <c r="J73" s="1">
@@ -19054,7 +19054,7 @@
         <v>-2.5265274936695655E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:66">
+    <row r="74" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>10</v>
       </c>
@@ -19317,7 +19317,7 @@
         <v>-2.5332541167705173E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:66">
+    <row r="75" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>11</v>
       </c>
@@ -19580,7 +19580,7 @@
         <v>-2.5327733940423689E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:66">
+    <row r="76" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>42</v>
       </c>
@@ -19843,7 +19843,7 @@
         <v>-2.5476999232319818E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:66">
+    <row r="77" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>13</v>
       </c>
@@ -20106,7 +20106,7 @@
         <v>-2.5496096269050522E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:66">
+    <row r="78" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>14</v>
       </c>
@@ -20369,7 +20369,7 @@
         <v>-2.5434366112232179E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:66">
+    <row r="79" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>15</v>
       </c>
@@ -20632,7 +20632,7 @@
         <v>-2.5335663246534275E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:66">
+    <row r="80" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>16</v>
       </c>
@@ -20895,7 +20895,7 @@
         <v>-2.543527756530346E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:66">
+    <row r="81" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>17</v>
       </c>
@@ -21158,7 +21158,7 @@
         <v>-2.5276563407196986E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:66">
+    <row r="82" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>18</v>
       </c>
@@ -21421,7 +21421,7 @@
         <v>-2.5358894966832531E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:66">
+    <row r="83" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>19</v>
       </c>
@@ -21684,7 +21684,7 @@
         <v>-2.5367095288272535E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:66">
+    <row r="84" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A84" s="9" t="s">
         <v>43</v>
       </c>
@@ -21709,7 +21709,7 @@
         <v>-1.4605159022990324E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:66">
+    <row r="85" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A85" s="9" t="s">
         <v>44</v>
       </c>
@@ -21888,13 +21888,13 @@
         <v>-2.5386091767948546E-3</v>
       </c>
     </row>
-    <row r="86" spans="1:66" ht="17.399999999999999">
+    <row r="86" spans="1:66" ht="18" x14ac:dyDescent="0.2">
       <c r="A86" s="23" t="s">
         <v>45</v>
       </c>
       <c r="B86" s="9"/>
     </row>
-    <row r="87" spans="1:66">
+    <row r="87" spans="1:66" x14ac:dyDescent="0.2">
       <c r="D87" s="9" t="s">
         <v>46</v>
       </c>
@@ -21906,7 +21906,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="88" spans="1:66" ht="49.5" customHeight="1">
+    <row r="88" spans="1:66" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C88" s="31">
         <v>40161</v>
       </c>
@@ -21941,7 +21941,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="89" spans="1:66">
+    <row r="89" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A89" s="16" t="s">
         <v>8</v>
       </c>
@@ -21990,7 +21990,7 @@
         <v>0.99939145670705609</v>
       </c>
     </row>
-    <row r="90" spans="1:66">
+    <row r="90" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A90" s="19" t="s">
         <v>56</v>
       </c>
@@ -22039,7 +22039,7 @@
         <v>0.99586221909432393</v>
       </c>
     </row>
-    <row r="91" spans="1:66">
+    <row r="91" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A91" s="16" t="s">
         <v>10</v>
       </c>
@@ -22088,7 +22088,7 @@
         <v>0.99973923711959634</v>
       </c>
     </row>
-    <row r="92" spans="1:66">
+    <row r="92" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A92" s="16" t="s">
         <v>11</v>
       </c>
@@ -22137,7 +22137,7 @@
         <v>0.99943590989950637</v>
       </c>
     </row>
-    <row r="93" spans="1:66">
+    <row r="93" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A93" s="16" t="s">
         <v>42</v>
       </c>
@@ -22186,7 +22186,7 @@
         <v>0.99984826875815802</v>
       </c>
     </row>
-    <row r="94" spans="1:66">
+    <row r="94" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A94" s="16" t="s">
         <v>13</v>
       </c>
@@ -22235,7 +22235,7 @@
         <v>1.0001152495611993</v>
       </c>
     </row>
-    <row r="95" spans="1:66">
+    <row r="95" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A95" s="16" t="s">
         <v>14</v>
       </c>
@@ -22284,7 +22284,7 @@
         <v>1.0004163806580109</v>
       </c>
     </row>
-    <row r="96" spans="1:66">
+    <row r="96" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A96" s="16" t="s">
         <v>15</v>
       </c>
@@ -22333,7 +22333,7 @@
         <v>0.99911994590802844</v>
       </c>
     </row>
-    <row r="97" spans="1:30">
+    <row r="97" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A97" s="16" t="s">
         <v>16</v>
       </c>
@@ -22382,7 +22382,7 @@
         <v>0.9995136617185042</v>
       </c>
     </row>
-    <row r="98" spans="1:30">
+    <row r="98" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A98" s="16" t="s">
         <v>17</v>
       </c>
@@ -22431,7 +22431,7 @@
         <v>0.99946076656726779</v>
       </c>
     </row>
-    <row r="99" spans="1:30">
+    <row r="99" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A99" s="16" t="s">
         <v>18</v>
       </c>
@@ -22480,7 +22480,7 @@
         <v>0.99899746798520295</v>
       </c>
     </row>
-    <row r="100" spans="1:30">
+    <row r="100" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A100" s="16" t="s">
         <v>19</v>
       </c>
@@ -22529,7 +22529,7 @@
         <v>1.0005953791714304</v>
       </c>
     </row>
-    <row r="101" spans="1:30">
+    <row r="101" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A101" s="16" t="s">
         <v>20</v>
       </c>
@@ -22571,7 +22571,7 @@
         <v>9.9973976415049659</v>
       </c>
     </row>
-    <row r="102" spans="1:30">
+    <row r="102" spans="1:30" x14ac:dyDescent="0.2">
       <c r="E102" s="41">
         <v>1.0435000000000001</v>
       </c>
@@ -22579,7 +22579,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="103" spans="1:30">
+    <row r="103" spans="1:30" x14ac:dyDescent="0.2">
       <c r="D103" s="41"/>
       <c r="E103">
         <v>7971000</v>
@@ -22588,7 +22588,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="104" spans="1:30">
+    <row r="104" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
         <v>59</v>
       </c>
@@ -22597,7 +22597,7 @@
         <v>0.99800089005360482</v>
       </c>
     </row>
-    <row r="105" spans="1:30" ht="17.399999999999999">
+    <row r="105" spans="1:30" ht="18" x14ac:dyDescent="0.2">
       <c r="A105" s="23" t="s">
         <v>60</v>
       </c>
@@ -22605,7 +22605,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="106" spans="1:30">
+    <row r="106" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>62</v>
       </c>
@@ -22653,7 +22653,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="107" spans="1:30">
+    <row r="107" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B107" s="6"/>
       <c r="F107" s="6"/>
       <c r="H107" s="30"/>
@@ -22710,7 +22710,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="108" spans="1:30" s="43" customFormat="1">
+    <row r="108" spans="1:30" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A108" s="43" t="s">
         <v>8</v>
       </c>
@@ -22827,7 +22827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:30" s="43" customFormat="1">
+    <row r="109" spans="1:30" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A109" s="43" t="s">
         <v>9</v>
       </c>
@@ -22944,7 +22944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:30" s="43" customFormat="1">
+    <row r="110" spans="1:30" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A110" s="43" t="s">
         <v>10</v>
       </c>
@@ -23061,7 +23061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:30" s="43" customFormat="1">
+    <row r="111" spans="1:30" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A111" s="43" t="s">
         <v>11</v>
       </c>
@@ -23178,7 +23178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:30" s="43" customFormat="1">
+    <row r="112" spans="1:30" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A112" s="43" t="s">
         <v>90</v>
       </c>
@@ -23295,7 +23295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:30" s="43" customFormat="1">
+    <row r="113" spans="1:30" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A113" s="43" t="s">
         <v>13</v>
       </c>
@@ -23412,7 +23412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:30" s="43" customFormat="1">
+    <row r="114" spans="1:30" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A114" s="43" t="s">
         <v>14</v>
       </c>
@@ -23529,7 +23529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:30" s="43" customFormat="1">
+    <row r="115" spans="1:30" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A115" s="43" t="s">
         <v>15</v>
       </c>
@@ -23646,7 +23646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:30" s="43" customFormat="1">
+    <row r="116" spans="1:30" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A116" s="43" t="s">
         <v>16</v>
       </c>
@@ -23763,7 +23763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:30" s="43" customFormat="1">
+    <row r="117" spans="1:30" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A117" s="43" t="s">
         <v>17</v>
       </c>
@@ -23880,7 +23880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:30" s="43" customFormat="1">
+    <row r="118" spans="1:30" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A118" s="43" t="s">
         <v>18</v>
       </c>
@@ -23997,7 +23997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:30" s="43" customFormat="1">
+    <row r="119" spans="1:30" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A119" s="43" t="s">
         <v>91</v>
       </c>
@@ -24114,7 +24114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:30">
+    <row r="120" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B120" s="37"/>
       <c r="C120" s="7"/>
       <c r="E120" s="41"/>
@@ -24134,7 +24134,7 @@
       <c r="Y120" s="54"/>
       <c r="Z120" s="54"/>
     </row>
-    <row r="121" spans="1:30" s="43" customFormat="1">
+    <row r="121" spans="1:30" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B121" s="45">
         <f>SUM(B108:B119)</f>
         <v>55.378945693874201</v>
@@ -24183,7 +24183,7 @@
         <v>1.9858427295232395E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:30" s="43" customFormat="1">
+    <row r="122" spans="1:30" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B122" s="56"/>
       <c r="F122" s="56"/>
       <c r="G122" s="43" t="s">
@@ -24204,7 +24204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:30" s="43" customFormat="1">
+    <row r="123" spans="1:30" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B123" s="56"/>
       <c r="F123" s="56"/>
       <c r="G123" s="43" t="s">
@@ -24226,7 +24226,7 @@
         <v>999.99999999999989</v>
       </c>
     </row>
-    <row r="124" spans="1:30" s="43" customFormat="1">
+    <row r="124" spans="1:30" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A124" s="43" t="s">
         <v>96</v>
       </c>
@@ -24248,7 +24248,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="125" spans="1:30" s="43" customFormat="1">
+    <row r="125" spans="1:30" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A125" s="43" t="s">
         <v>99</v>
       </c>
@@ -24284,7 +24284,7 @@
         <v>999.99999999999989</v>
       </c>
     </row>
-    <row r="126" spans="1:30" s="43" customFormat="1">
+    <row r="126" spans="1:30" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B126" s="56"/>
       <c r="F126" s="56"/>
       <c r="H126" s="57"/>
@@ -24301,7 +24301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:30" s="43" customFormat="1">
+    <row r="127" spans="1:30" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A127" s="43" t="s">
         <v>100</v>
       </c>
@@ -24339,7 +24339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:30" s="43" customFormat="1">
+    <row r="128" spans="1:30" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A128" s="43" t="s">
         <v>100</v>
       </c>
@@ -24374,7 +24374,7 @@
       <c r="R128" s="56"/>
       <c r="S128" s="56"/>
     </row>
-    <row r="129" spans="1:33">
+    <row r="129" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A129" s="63"/>
       <c r="B129" s="64">
         <v>2015</v>
@@ -24386,7 +24386,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="130" spans="1:33" s="2" customFormat="1">
+    <row r="130" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A130" s="67" t="s">
         <v>103</v>
       </c>
@@ -24394,7 +24394,7 @@
       <c r="C130" s="68"/>
       <c r="D130" s="69"/>
     </row>
-    <row r="131" spans="1:33" ht="13.5" customHeight="1">
+    <row r="131" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="70" t="s">
         <v>104</v>
       </c>
@@ -24447,7 +24447,7 @@
         <v>2115</v>
       </c>
     </row>
-    <row r="132" spans="1:33">
+    <row r="132" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A132" s="70" t="s">
         <v>105</v>
       </c>
@@ -24513,7 +24513,7 @@
         <v>2.7969113101572921E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:33">
+    <row r="133" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A133" s="70" t="s">
         <v>106</v>
       </c>
@@ -24593,7 +24593,7 @@
       <c r="AF133" s="2"/>
       <c r="AG133" s="2"/>
     </row>
-    <row r="134" spans="1:33">
+    <row r="134" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A134" s="70" t="s">
         <v>107</v>
       </c>
@@ -24659,7 +24659,7 @@
         <v>3.475984762518456E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:33">
+    <row r="135" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A135" s="70"/>
       <c r="B135" s="71"/>
       <c r="C135" s="71"/>
@@ -24718,7 +24718,7 @@
       </c>
       <c r="R135" s="2"/>
     </row>
-    <row r="136" spans="1:33">
+    <row r="136" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A136" s="73"/>
       <c r="B136" s="74"/>
       <c r="C136" s="74"/>
@@ -24792,7 +24792,7 @@
       <c r="AF136" s="2"/>
       <c r="AG136" s="2"/>
     </row>
-    <row r="138" spans="1:33">
+    <row r="138" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>62</v>
       </c>
@@ -24833,7 +24833,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="139" spans="1:33">
+    <row r="139" spans="1:33" x14ac:dyDescent="0.2">
       <c r="C139" s="6"/>
       <c r="D139" s="6"/>
       <c r="E139" s="6"/>
@@ -24847,7 +24847,7 @@
       <c r="M139" s="6"/>
       <c r="N139" s="6"/>
     </row>
-    <row r="140" spans="1:33" s="30" customFormat="1">
+    <row r="140" spans="1:33" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A140" s="42" t="s">
         <v>63</v>
       </c>
@@ -24900,7 +24900,7 @@
         <v>2.6191887369437761</v>
       </c>
     </row>
-    <row r="141" spans="1:33">
+    <row r="141" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A141" s="9" t="s">
         <v>59</v>
       </c>
@@ -24953,7 +24953,7 @@
         <v>937.19556697899202</v>
       </c>
     </row>
-    <row r="142" spans="1:33">
+    <row r="142" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A142" s="9" t="s">
         <v>108</v>
       </c>
@@ -25006,7 +25006,7 @@
         <v>7.7765473111546274E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:33">
+    <row r="143" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A143" s="9" t="s">
         <v>80</v>
       </c>
@@ -25059,7 +25059,7 @@
         <v>4.4201869312950182</v>
       </c>
     </row>
-    <row r="144" spans="1:33">
+    <row r="144" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A144" s="9" t="s">
         <v>78</v>
       </c>
@@ -25112,7 +25112,7 @@
         <v>1.7549043305648544</v>
       </c>
     </row>
-    <row r="145" spans="1:26">
+    <row r="145" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A145" s="9" t="s">
         <v>81</v>
       </c>
@@ -25165,7 +25165,7 @@
         <v>0.24387582996705415</v>
       </c>
     </row>
-    <row r="146" spans="1:26">
+    <row r="146" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A146" s="9" t="s">
         <v>109</v>
       </c>
@@ -25218,7 +25218,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="147" spans="1:26">
+    <row r="147" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A147" s="9" t="s">
         <v>110</v>
       </c>
@@ -25271,7 +25271,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="148" spans="1:26">
+    <row r="148" spans="1:26" x14ac:dyDescent="0.2">
       <c r="O148" s="12"/>
       <c r="P148" s="12"/>
       <c r="Q148" s="12"/>
@@ -25285,7 +25285,7 @@
       <c r="Y148" s="12"/>
       <c r="Z148" s="12"/>
     </row>
-    <row r="149" spans="1:26">
+    <row r="149" spans="1:26" x14ac:dyDescent="0.2">
       <c r="C149" s="12"/>
       <c r="D149" s="12"/>
       <c r="E149" s="12"/>
@@ -25299,7 +25299,7 @@
       <c r="M149" s="12"/>
       <c r="N149" s="12"/>
     </row>
-    <row r="150" spans="1:26">
+    <row r="150" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A150" s="9" t="s">
         <v>111</v>
       </c>
@@ -25356,7 +25356,7 @@
         <v>2504.2063968864404</v>
       </c>
     </row>
-    <row r="153" spans="1:26" ht="19.8">
+    <row r="153" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A153" s="78" t="s">
         <v>112</v>
       </c>
@@ -25364,46 +25364,46 @@
         <v>113</v>
       </c>
     </row>
-    <row r="154" spans="1:26" s="23" customFormat="1" ht="17.399999999999999">
+    <row r="154" spans="1:26" s="23" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A154" s="23" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="155" spans="1:26" s="23" customFormat="1" ht="17.399999999999999">
+    <row r="155" spans="1:26" s="23" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A155" s="23" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="156" spans="1:26" s="23" customFormat="1" ht="17.399999999999999">
+    <row r="156" spans="1:26" s="23" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A156" s="23" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="157" spans="1:26" s="23" customFormat="1" ht="17.399999999999999">
+    <row r="157" spans="1:26" s="23" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A157" s="23" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="158" spans="1:26" s="23" customFormat="1" ht="17.399999999999999"/>
-    <row r="159" spans="1:26" s="23" customFormat="1" ht="17.399999999999999"/>
-    <row r="160" spans="1:26" s="23" customFormat="1" ht="17.399999999999999">
+    <row r="158" spans="1:26" s="23" customFormat="1" ht="18" x14ac:dyDescent="0.2"/>
+    <row r="159" spans="1:26" s="23" customFormat="1" ht="18" x14ac:dyDescent="0.2"/>
+    <row r="160" spans="1:26" s="23" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A160" s="23" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="161" spans="1:19" s="23" customFormat="1" ht="17.399999999999999">
+    <row r="161" spans="1:19" s="23" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A161" s="23" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="162" spans="1:19" s="23" customFormat="1" ht="17.399999999999999"/>
-    <row r="163" spans="1:19" s="23" customFormat="1" ht="17.399999999999999">
+    <row r="162" spans="1:19" s="23" customFormat="1" ht="18" x14ac:dyDescent="0.2"/>
+    <row r="163" spans="1:19" s="23" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A163" s="23" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="164" spans="1:19" s="23" customFormat="1" ht="17.25" customHeight="1"/>
-    <row r="165" spans="1:19" s="16" customFormat="1" ht="17.25" customHeight="1">
+    <row r="164" spans="1:19" s="23" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="165" spans="1:19" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="80" t="s">
         <v>121</v>
       </c>
@@ -25415,13 +25415,13 @@
       <c r="G165" s="81"/>
       <c r="H165" s="81"/>
     </row>
-    <row r="166" spans="1:19" s="16" customFormat="1" ht="17.25" customHeight="1"/>
-    <row r="167" spans="1:19" s="16" customFormat="1" ht="17.25" customHeight="1">
+    <row r="166" spans="1:19" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="167" spans="1:19" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="P167" s="16" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="168" spans="1:19" s="16" customFormat="1" ht="36" customHeight="1">
+    <row r="168" spans="1:19" s="16" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C168" s="16" t="s">
         <v>123</v>
       </c>
@@ -25459,7 +25459,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="169" spans="1:19" s="16" customFormat="1" ht="17.25" customHeight="1">
+    <row r="169" spans="1:19" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B169" s="16" t="s">
         <v>8</v>
       </c>
@@ -25525,7 +25525,7 @@
         <v>68030.010240009011</v>
       </c>
     </row>
-    <row r="170" spans="1:19" s="16" customFormat="1" ht="17.25" customHeight="1">
+    <row r="170" spans="1:19" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B170" s="16" t="s">
         <v>56</v>
       </c>
@@ -25584,7 +25584,7 @@
         <v>-1190.0914153813032</v>
       </c>
     </row>
-    <row r="171" spans="1:19" s="16" customFormat="1" ht="17.25" customHeight="1">
+    <row r="171" spans="1:19" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B171" s="16" t="s">
         <v>10</v>
       </c>
@@ -25643,7 +25643,7 @@
         <v>-329.12911021178326</v>
       </c>
     </row>
-    <row r="172" spans="1:19" s="16" customFormat="1" ht="17.25" customHeight="1">
+    <row r="172" spans="1:19" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B172" s="16" t="s">
         <v>11</v>
       </c>
@@ -25702,7 +25702,7 @@
         <v>-34.076238157336846</v>
       </c>
     </row>
-    <row r="173" spans="1:19" s="16" customFormat="1" ht="17.25" customHeight="1">
+    <row r="173" spans="1:19" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B173" s="16" t="s">
         <v>42</v>
       </c>
@@ -25761,7 +25761,7 @@
         <v>6.4007131154632475</v>
       </c>
     </row>
-    <row r="174" spans="1:19" s="16" customFormat="1" ht="17.25" customHeight="1">
+    <row r="174" spans="1:19" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B174" s="16" t="s">
         <v>13</v>
       </c>
@@ -25820,7 +25820,7 @@
         <v>272.42355548616791</v>
       </c>
     </row>
-    <row r="175" spans="1:19" s="16" customFormat="1" ht="17.25" customHeight="1">
+    <row r="175" spans="1:19" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B175" s="16" t="s">
         <v>14</v>
       </c>
@@ -25879,7 +25879,7 @@
         <v>121.65263232935504</v>
       </c>
     </row>
-    <row r="176" spans="1:19" s="16" customFormat="1" ht="17.25" customHeight="1">
+    <row r="176" spans="1:19" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B176" s="16" t="s">
         <v>15</v>
       </c>
@@ -25938,7 +25938,7 @@
         <v>-79.157194445829305</v>
       </c>
     </row>
-    <row r="177" spans="2:17" s="16" customFormat="1" ht="17.25" customHeight="1">
+    <row r="177" spans="2:17" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B177" s="16" t="s">
         <v>16</v>
       </c>
@@ -25997,7 +25997,7 @@
         <v>76.683017337879335</v>
       </c>
     </row>
-    <row r="178" spans="2:17" s="16" customFormat="1" ht="17.25" customHeight="1">
+    <row r="178" spans="2:17" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B178" s="16" t="s">
         <v>17</v>
       </c>
@@ -26056,7 +26056,7 @@
         <v>14.029636873577545</v>
       </c>
     </row>
-    <row r="179" spans="2:17" s="16" customFormat="1" ht="17.25" customHeight="1">
+    <row r="179" spans="2:17" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B179" s="16" t="s">
         <v>18</v>
       </c>
@@ -26115,7 +26115,7 @@
         <v>-401.95662608894492</v>
       </c>
     </row>
-    <row r="180" spans="2:17" s="16" customFormat="1" ht="17.25" customHeight="1">
+    <row r="180" spans="2:17" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B180" s="16" t="s">
         <v>134</v>
       </c>
@@ -26174,7 +26174,7 @@
         <v>126.98709766030743</v>
       </c>
     </row>
-    <row r="181" spans="2:17" s="16" customFormat="1" ht="17.25" customHeight="1">
+    <row r="181" spans="2:17" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F181" s="16">
         <v>0</v>
       </c>
@@ -26190,14 +26190,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="2:17" s="16" customFormat="1" ht="17.25" customHeight="1"/>
-    <row r="183" spans="2:17" s="16" customFormat="1" ht="17.25" customHeight="1"/>
-    <row r="184" spans="2:17" s="16" customFormat="1" ht="17.25" customHeight="1">
+    <row r="182" spans="2:17" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="183" spans="2:17" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="184" spans="2:17" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I184" s="16" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="185" spans="2:17" ht="17.399999999999999">
+    <row r="185" spans="2:17" ht="18" x14ac:dyDescent="0.2">
       <c r="I185" s="85" t="s">
         <v>136</v>
       </c>
@@ -26205,7 +26205,7 @@
       <c r="K185" s="86"/>
       <c r="L185" s="86"/>
     </row>
-    <row r="186" spans="2:17" ht="17.399999999999999">
+    <row r="186" spans="2:17" ht="18" x14ac:dyDescent="0.2">
       <c r="I186" s="85" t="s">
         <v>137</v>
       </c>
@@ -26213,7 +26213,7 @@
       <c r="K186" s="86"/>
       <c r="L186" s="86"/>
     </row>
-    <row r="187" spans="2:17" ht="17.399999999999999">
+    <row r="187" spans="2:17" ht="18" x14ac:dyDescent="0.2">
       <c r="I187" s="85" t="s">
         <v>138</v>
       </c>
@@ -26221,7 +26221,7 @@
       <c r="K187" s="86"/>
       <c r="L187" s="86"/>
     </row>
-    <row r="188" spans="2:17" ht="17.399999999999999">
+    <row r="188" spans="2:17" ht="18" x14ac:dyDescent="0.2">
       <c r="I188" s="85" t="s">
         <v>139</v>
       </c>
@@ -26230,10 +26230,10 @@
       <c r="L188" s="86"/>
       <c r="O188" s="43"/>
     </row>
-    <row r="189" spans="2:17">
+    <row r="189" spans="2:17" x14ac:dyDescent="0.2">
       <c r="O189" s="43"/>
     </row>
-    <row r="190" spans="2:17" ht="17.399999999999999">
+    <row r="190" spans="2:17" ht="18" x14ac:dyDescent="0.2">
       <c r="I190" s="85" t="s">
         <v>140</v>
       </c>
@@ -26242,13 +26242,13 @@
       <c r="L190" s="86"/>
       <c r="O190" s="43"/>
     </row>
-    <row r="191" spans="2:17">
+    <row r="191" spans="2:17" x14ac:dyDescent="0.2">
       <c r="O191" s="43"/>
     </row>
-    <row r="192" spans="2:17">
+    <row r="192" spans="2:17" x14ac:dyDescent="0.2">
       <c r="O192" s="43"/>
     </row>
-    <row r="193" spans="1:61" ht="17.399999999999999">
+    <row r="193" spans="1:61" ht="18" x14ac:dyDescent="0.2">
       <c r="A193" s="85" t="s">
         <v>141</v>
       </c>
@@ -26260,42 +26260,42 @@
       <c r="G193" s="86"/>
       <c r="H193" s="86"/>
     </row>
-    <row r="194" spans="1:61">
+    <row r="194" spans="1:61" x14ac:dyDescent="0.2">
       <c r="O194" s="43"/>
     </row>
-    <row r="195" spans="1:61" ht="17.399999999999999">
+    <row r="195" spans="1:61" ht="18" x14ac:dyDescent="0.2">
       <c r="A195" s="23" t="s">
         <v>142</v>
       </c>
       <c r="O195" s="43"/>
     </row>
-    <row r="196" spans="1:61" ht="17.399999999999999">
+    <row r="196" spans="1:61" ht="18" x14ac:dyDescent="0.2">
       <c r="A196" s="23"/>
       <c r="O196" s="43"/>
     </row>
-    <row r="197" spans="1:61" s="86" customFormat="1" ht="17.399999999999999">
+    <row r="197" spans="1:61" s="86" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A197" s="85" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="198" spans="1:61" s="86" customFormat="1" ht="17.399999999999999">
+    <row r="198" spans="1:61" s="86" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A198" s="85" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="199" spans="1:61" ht="17.399999999999999">
+    <row r="199" spans="1:61" ht="18" x14ac:dyDescent="0.2">
       <c r="A199" s="23"/>
       <c r="O199" s="43"/>
     </row>
-    <row r="200" spans="1:61">
+    <row r="200" spans="1:61" x14ac:dyDescent="0.2">
       <c r="O200" s="43"/>
     </row>
-    <row r="201" spans="1:61" s="88" customFormat="1" ht="12.9">
+    <row r="201" spans="1:61" s="88" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A201" s="88" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="202" spans="1:61" s="91" customFormat="1" ht="18" customHeight="1">
+    <row r="202" spans="1:61" s="91" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" s="89"/>
       <c r="B202" s="90">
         <v>2005</v>
@@ -26478,8 +26478,8 @@
         <v>2595</v>
       </c>
     </row>
-    <row r="203" spans="1:61" s="88" customFormat="1" ht="12.9"/>
-    <row r="204" spans="1:61" s="92" customFormat="1">
+    <row r="203" spans="1:61" s="88" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
+    <row r="204" spans="1:61" s="92" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A204" s="92" t="s">
         <v>8</v>
       </c>
@@ -26724,7 +26724,7 @@
         <v>846.93813321666664</v>
       </c>
     </row>
-    <row r="205" spans="1:61" s="92" customFormat="1">
+    <row r="205" spans="1:61" s="92" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A205" s="92" t="s">
         <v>56</v>
       </c>
@@ -26969,7 +26969,7 @@
         <v>659.13303651849617</v>
       </c>
     </row>
-    <row r="206" spans="1:61" s="92" customFormat="1">
+    <row r="206" spans="1:61" s="92" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A206" s="92" t="s">
         <v>10</v>
       </c>
@@ -27214,7 +27214,7 @@
         <v>777.62581677762444</v>
       </c>
     </row>
-    <row r="207" spans="1:61" s="92" customFormat="1">
+    <row r="207" spans="1:61" s="92" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A207" s="92" t="s">
         <v>11</v>
       </c>
@@ -27459,7 +27459,7 @@
         <v>577.28859338189875</v>
       </c>
     </row>
-    <row r="208" spans="1:61" s="92" customFormat="1">
+    <row r="208" spans="1:61" s="92" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A208" s="92" t="s">
         <v>42</v>
       </c>
@@ -27704,7 +27704,7 @@
         <v>572.25361530575242</v>
       </c>
     </row>
-    <row r="209" spans="1:61" s="92" customFormat="1">
+    <row r="209" spans="1:61" s="92" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A209" s="92" t="s">
         <v>13</v>
       </c>
@@ -27949,7 +27949,7 @@
         <v>194.58590362590155</v>
       </c>
     </row>
-    <row r="210" spans="1:61" s="92" customFormat="1">
+    <row r="210" spans="1:61" s="92" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A210" s="92" t="s">
         <v>14</v>
       </c>
@@ -28194,7 +28194,7 @@
         <v>397.07887874790759</v>
       </c>
     </row>
-    <row r="211" spans="1:61" s="92" customFormat="1">
+    <row r="211" spans="1:61" s="92" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A211" s="92" t="s">
         <v>15</v>
       </c>
@@ -28439,7 +28439,7 @@
         <v>436.74518251427463</v>
       </c>
     </row>
-    <row r="212" spans="1:61" s="92" customFormat="1">
+    <row r="212" spans="1:61" s="92" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A212" s="92" t="s">
         <v>16</v>
       </c>
@@ -28684,7 +28684,7 @@
         <v>253.84016537361276</v>
       </c>
     </row>
-    <row r="213" spans="1:61" s="92" customFormat="1">
+    <row r="213" spans="1:61" s="92" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A213" s="92" t="s">
         <v>17</v>
       </c>
@@ -28929,7 +28929,7 @@
         <v>648.68639135878993</v>
       </c>
     </row>
-    <row r="214" spans="1:61" s="92" customFormat="1">
+    <row r="214" spans="1:61" s="92" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A214" s="92" t="s">
         <v>18</v>
       </c>
@@ -29174,7 +29174,7 @@
         <v>601.29683315672207</v>
       </c>
     </row>
-    <row r="215" spans="1:61" s="92" customFormat="1">
+    <row r="215" spans="1:61" s="92" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A215" s="92" t="s">
         <v>134</v>
       </c>
@@ -29419,7 +29419,7 @@
         <v>234.83576868876483</v>
       </c>
     </row>
-    <row r="216" spans="1:61" s="94" customFormat="1">
+    <row r="216" spans="1:61" s="94" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C216" s="95"/>
       <c r="D216" s="95"/>
       <c r="E216" s="95"/>
@@ -29480,7 +29480,7 @@
       <c r="BH216" s="95"/>
       <c r="BI216" s="95"/>
     </row>
-    <row r="217" spans="1:61" s="94" customFormat="1">
+    <row r="217" spans="1:61" s="94" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A217" s="96" t="s">
         <v>146</v>
       </c>
@@ -29553,17 +29553,17 @@
       <c r="BH217" s="97"/>
       <c r="BI217" s="97"/>
     </row>
-    <row r="218" spans="1:61" s="99" customFormat="1">
+    <row r="218" spans="1:61" s="99" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A218" s="98" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="219" spans="1:61" s="99" customFormat="1">
+    <row r="219" spans="1:61" s="99" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B219" s="100" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="220" spans="1:61" s="103" customFormat="1">
+    <row r="220" spans="1:61" s="103" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A220" s="101" t="s">
         <v>8</v>
       </c>
@@ -29808,7 +29808,7 @@
         <v>24647.764226475865</v>
       </c>
     </row>
-    <row r="221" spans="1:61" s="103" customFormat="1">
+    <row r="221" spans="1:61" s="103" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A221" s="101" t="s">
         <v>56</v>
       </c>
@@ -30053,7 +30053,7 @@
         <v>16922.30893494092</v>
       </c>
     </row>
-    <row r="222" spans="1:61" s="103" customFormat="1">
+    <row r="222" spans="1:61" s="103" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A222" s="101" t="s">
         <v>10</v>
       </c>
@@ -30298,7 +30298,7 @@
         <v>21684.829198899166</v>
       </c>
     </row>
-    <row r="223" spans="1:61" s="103" customFormat="1">
+    <row r="223" spans="1:61" s="103" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A223" s="101" t="s">
         <v>11</v>
       </c>
@@ -30543,7 +30543,7 @@
         <v>13870.415296971858</v>
       </c>
     </row>
-    <row r="224" spans="1:61" s="103" customFormat="1">
+    <row r="224" spans="1:61" s="103" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A224" s="101" t="s">
         <v>42</v>
       </c>
@@ -30788,7 +30788,7 @@
         <v>13689.349692416561</v>
       </c>
     </row>
-    <row r="225" spans="1:122" s="103" customFormat="1">
+    <row r="225" spans="1:122" s="103" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A225" s="101" t="s">
         <v>13</v>
       </c>
@@ -31033,7 +31033,7 @@
         <v>2714.3576032763876</v>
       </c>
     </row>
-    <row r="226" spans="1:122" s="103" customFormat="1">
+    <row r="226" spans="1:122" s="103" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A226" s="101" t="s">
         <v>14</v>
       </c>
@@ -31278,7 +31278,7 @@
         <v>7912.5265505057987</v>
       </c>
     </row>
-    <row r="227" spans="1:122" s="103" customFormat="1">
+    <row r="227" spans="1:122" s="103" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A227" s="101" t="s">
         <v>15</v>
       </c>
@@ -31523,7 +31523,7 @@
         <v>9127.2970472066718</v>
       </c>
     </row>
-    <row r="228" spans="1:122" s="103" customFormat="1">
+    <row r="228" spans="1:122" s="103" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A228" s="101" t="s">
         <v>16</v>
       </c>
@@ -31768,7 +31768,7 @@
         <v>4044.2734564498519</v>
       </c>
     </row>
-    <row r="229" spans="1:122" s="103" customFormat="1">
+    <row r="229" spans="1:122" s="103" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A229" s="101" t="s">
         <v>17</v>
       </c>
@@ -32013,7 +32013,7 @@
         <v>16521.602937895797</v>
       </c>
     </row>
-    <row r="230" spans="1:122" s="103" customFormat="1">
+    <row r="230" spans="1:122" s="103" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A230" s="101" t="s">
         <v>18</v>
       </c>
@@ -32258,7 +32258,7 @@
         <v>14744.612886999375</v>
       </c>
     </row>
-    <row r="231" spans="1:122" s="103" customFormat="1">
+    <row r="231" spans="1:122" s="103" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A231" s="101" t="s">
         <v>134</v>
       </c>
@@ -32503,7 +32503,7 @@
         <v>3598.7060158184095</v>
       </c>
     </row>
-    <row r="232" spans="1:122" s="99" customFormat="1">
+    <row r="232" spans="1:122" s="99" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A232" s="104" t="s">
         <v>148</v>
       </c>
@@ -32512,7 +32512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:122" s="99" customFormat="1">
+    <row r="233" spans="1:122" s="99" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B233" s="99" t="s">
         <v>124</v>
       </c>
@@ -32520,7 +32520,7 @@
       <c r="D233" s="105"/>
       <c r="DR233" s="100"/>
     </row>
-    <row r="234" spans="1:122" s="106" customFormat="1">
+    <row r="234" spans="1:122" s="106" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A234" s="106" t="s">
         <v>8</v>
       </c>
@@ -32706,7 +32706,7 @@
       </c>
       <c r="DR234" s="107"/>
     </row>
-    <row r="235" spans="1:122" s="106" customFormat="1">
+    <row r="235" spans="1:122" s="106" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A235" s="106" t="s">
         <v>56</v>
       </c>
@@ -32892,7 +32892,7 @@
       </c>
       <c r="DR235" s="107"/>
     </row>
-    <row r="236" spans="1:122" s="106" customFormat="1">
+    <row r="236" spans="1:122" s="106" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A236" s="106" t="s">
         <v>10</v>
       </c>
@@ -33078,7 +33078,7 @@
       </c>
       <c r="DR236" s="107"/>
     </row>
-    <row r="237" spans="1:122" s="106" customFormat="1">
+    <row r="237" spans="1:122" s="106" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A237" s="106" t="s">
         <v>11</v>
       </c>
@@ -33264,7 +33264,7 @@
       </c>
       <c r="DR237" s="107"/>
     </row>
-    <row r="238" spans="1:122" s="106" customFormat="1">
+    <row r="238" spans="1:122" s="106" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A238" s="106" t="s">
         <v>42</v>
       </c>
@@ -33450,7 +33450,7 @@
       </c>
       <c r="DR238" s="107"/>
     </row>
-    <row r="239" spans="1:122" s="106" customFormat="1">
+    <row r="239" spans="1:122" s="106" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A239" s="106" t="s">
         <v>13</v>
       </c>
@@ -33636,7 +33636,7 @@
       </c>
       <c r="DR239" s="107"/>
     </row>
-    <row r="240" spans="1:122" s="106" customFormat="1">
+    <row r="240" spans="1:122" s="106" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A240" s="106" t="s">
         <v>14</v>
       </c>
@@ -33822,7 +33822,7 @@
       </c>
       <c r="DR240" s="107"/>
     </row>
-    <row r="241" spans="1:122" s="106" customFormat="1">
+    <row r="241" spans="1:122" s="106" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A241" s="106" t="s">
         <v>15</v>
       </c>
@@ -34008,7 +34008,7 @@
       </c>
       <c r="DR241" s="107"/>
     </row>
-    <row r="242" spans="1:122" s="106" customFormat="1">
+    <row r="242" spans="1:122" s="106" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A242" s="106" t="s">
         <v>16</v>
       </c>
@@ -34194,7 +34194,7 @@
       </c>
       <c r="DR242" s="107"/>
     </row>
-    <row r="243" spans="1:122" s="106" customFormat="1">
+    <row r="243" spans="1:122" s="106" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A243" s="106" t="s">
         <v>17</v>
       </c>
@@ -34380,7 +34380,7 @@
       </c>
       <c r="DR243" s="107"/>
     </row>
-    <row r="244" spans="1:122" s="106" customFormat="1">
+    <row r="244" spans="1:122" s="106" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A244" s="106" t="s">
         <v>18</v>
       </c>
@@ -34566,7 +34566,7 @@
       </c>
       <c r="DR244" s="107"/>
     </row>
-    <row r="245" spans="1:122" s="106" customFormat="1">
+    <row r="245" spans="1:122" s="106" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A245" s="106" t="s">
         <v>134</v>
       </c>
@@ -34752,16 +34752,16 @@
       </c>
       <c r="DR245" s="107"/>
     </row>
-    <row r="246" spans="1:122" s="99" customFormat="1">
+    <row r="246" spans="1:122" s="99" customFormat="1" x14ac:dyDescent="0.2">
       <c r="DR246" s="100"/>
     </row>
-    <row r="247" spans="1:122" s="99" customFormat="1">
+    <row r="247" spans="1:122" s="99" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A247" s="99" t="s">
         <v>149</v>
       </c>
       <c r="DR247" s="100"/>
     </row>
-    <row r="248" spans="1:122" s="99" customFormat="1">
+    <row r="248" spans="1:122" s="99" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A248" s="99" t="s">
         <v>8</v>
       </c>
@@ -35007,7 +35007,7 @@
       </c>
       <c r="DR248" s="100"/>
     </row>
-    <row r="249" spans="1:122" s="99" customFormat="1">
+    <row r="249" spans="1:122" s="99" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A249" s="99" t="s">
         <v>56</v>
       </c>
@@ -35253,7 +35253,7 @@
       </c>
       <c r="DR249" s="100"/>
     </row>
-    <row r="250" spans="1:122" s="99" customFormat="1">
+    <row r="250" spans="1:122" s="99" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A250" s="99" t="s">
         <v>10</v>
       </c>
@@ -35499,7 +35499,7 @@
       </c>
       <c r="DR250" s="100"/>
     </row>
-    <row r="251" spans="1:122" s="99" customFormat="1">
+    <row r="251" spans="1:122" s="99" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A251" s="99" t="s">
         <v>11</v>
       </c>
@@ -35745,7 +35745,7 @@
       </c>
       <c r="DR251" s="100"/>
     </row>
-    <row r="252" spans="1:122" s="99" customFormat="1">
+    <row r="252" spans="1:122" s="99" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A252" s="99" t="s">
         <v>42</v>
       </c>
@@ -35991,7 +35991,7 @@
       </c>
       <c r="DR252" s="100"/>
     </row>
-    <row r="253" spans="1:122" s="99" customFormat="1">
+    <row r="253" spans="1:122" s="99" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A253" s="99" t="s">
         <v>13</v>
       </c>
@@ -36056,7 +36056,7 @@
         <v>12.189870608531093</v>
       </c>
       <c r="Q253" s="99">
-        <f t="shared" ref="Q253:BT253" si="65">+(Q239/Q$234)/($B239/$B$234)</f>
+        <f t="shared" ref="Q253:BI253" si="65">+(Q239/Q$234)/($B239/$B$234)</f>
         <v>12.543067555440846</v>
       </c>
       <c r="R253" s="99">
@@ -36237,7 +36237,7 @@
       </c>
       <c r="DR253" s="100"/>
     </row>
-    <row r="254" spans="1:122" s="99" customFormat="1">
+    <row r="254" spans="1:122" s="99" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A254" s="99" t="s">
         <v>14</v>
       </c>
@@ -36483,7 +36483,7 @@
       </c>
       <c r="DR254" s="100"/>
     </row>
-    <row r="255" spans="1:122" s="99" customFormat="1">
+    <row r="255" spans="1:122" s="99" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A255" s="99" t="s">
         <v>15</v>
       </c>
@@ -36729,7 +36729,7 @@
       </c>
       <c r="DR255" s="100"/>
     </row>
-    <row r="256" spans="1:122" s="99" customFormat="1">
+    <row r="256" spans="1:122" s="99" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A256" s="99" t="s">
         <v>16</v>
       </c>
@@ -36975,7 +36975,7 @@
       </c>
       <c r="DR256" s="100"/>
     </row>
-    <row r="257" spans="1:122" s="99" customFormat="1">
+    <row r="257" spans="1:122" s="99" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A257" s="99" t="s">
         <v>17</v>
       </c>
@@ -37221,7 +37221,7 @@
       </c>
       <c r="DR257" s="100"/>
     </row>
-    <row r="258" spans="1:122" s="99" customFormat="1">
+    <row r="258" spans="1:122" s="99" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A258" s="99" t="s">
         <v>18</v>
       </c>
@@ -37286,7 +37286,7 @@
         <v>1.2896302101425554</v>
       </c>
       <c r="Q258" s="99">
-        <f t="shared" ref="Q258:BT258" si="67">+(Q244/Q$234)/($B244/$B$234)</f>
+        <f t="shared" ref="Q258:BI258" si="67">+(Q244/Q$234)/($B244/$B$234)</f>
         <v>1.2894225292736636</v>
       </c>
       <c r="R258" s="99">
@@ -37467,7 +37467,7 @@
       </c>
       <c r="DR258" s="100"/>
     </row>
-    <row r="259" spans="1:122" s="99" customFormat="1">
+    <row r="259" spans="1:122" s="99" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A259" s="99" t="s">
         <v>134</v>
       </c>
@@ -37713,16 +37713,16 @@
       </c>
       <c r="DR259" s="100"/>
     </row>
-    <row r="260" spans="1:122" s="108" customFormat="1">
+    <row r="260" spans="1:122" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="DR260" s="109"/>
     </row>
-    <row r="261" spans="1:122" s="108" customFormat="1">
+    <row r="261" spans="1:122" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A261" s="110" t="s">
         <v>150</v>
       </c>
       <c r="DR261" s="109"/>
     </row>
-    <row r="262" spans="1:122" s="108" customFormat="1">
+    <row r="262" spans="1:122" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A262" s="108" t="s">
         <v>8</v>
       </c>
@@ -37968,7 +37968,7 @@
       </c>
       <c r="DR262" s="109"/>
     </row>
-    <row r="263" spans="1:122" s="108" customFormat="1">
+    <row r="263" spans="1:122" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A263" s="108" t="s">
         <v>56</v>
       </c>
@@ -38214,7 +38214,7 @@
       </c>
       <c r="DR263" s="109"/>
     </row>
-    <row r="264" spans="1:122" s="108" customFormat="1">
+    <row r="264" spans="1:122" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A264" s="108" t="s">
         <v>10</v>
       </c>
@@ -38460,7 +38460,7 @@
       </c>
       <c r="DR264" s="109"/>
     </row>
-    <row r="265" spans="1:122" s="108" customFormat="1">
+    <row r="265" spans="1:122" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A265" s="108" t="s">
         <v>11</v>
       </c>
@@ -38706,7 +38706,7 @@
       </c>
       <c r="DR265" s="109"/>
     </row>
-    <row r="266" spans="1:122" s="108" customFormat="1">
+    <row r="266" spans="1:122" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A266" s="108" t="s">
         <v>42</v>
       </c>
@@ -38771,7 +38771,7 @@
         <v>0.15440158967945455</v>
       </c>
       <c r="Q266" s="108">
-        <f t="shared" ref="Q266:BW266" si="70">1/Q252</f>
+        <f t="shared" ref="Q266:BI266" si="70">1/Q252</f>
         <v>0.14542107669934692</v>
       </c>
       <c r="R266" s="108">
@@ -38952,7 +38952,7 @@
       </c>
       <c r="DR266" s="109"/>
     </row>
-    <row r="267" spans="1:122" s="108" customFormat="1">
+    <row r="267" spans="1:122" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A267" s="108" t="s">
         <v>13</v>
       </c>
@@ -39198,7 +39198,7 @@
       </c>
       <c r="DR267" s="109"/>
     </row>
-    <row r="268" spans="1:122" s="108" customFormat="1">
+    <row r="268" spans="1:122" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A268" s="108" t="s">
         <v>14</v>
       </c>
@@ -39444,7 +39444,7 @@
       </c>
       <c r="DR268" s="109"/>
     </row>
-    <row r="269" spans="1:122" s="108" customFormat="1">
+    <row r="269" spans="1:122" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A269" s="108" t="s">
         <v>15</v>
       </c>
@@ -39690,7 +39690,7 @@
       </c>
       <c r="DR269" s="109"/>
     </row>
-    <row r="270" spans="1:122" s="108" customFormat="1">
+    <row r="270" spans="1:122" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A270" s="108" t="s">
         <v>16</v>
       </c>
@@ -39936,7 +39936,7 @@
       </c>
       <c r="DR270" s="109"/>
     </row>
-    <row r="271" spans="1:122" s="108" customFormat="1">
+    <row r="271" spans="1:122" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A271" s="108" t="s">
         <v>17</v>
       </c>
@@ -40001,7 +40001,7 @@
         <v>0.19645208199540054</v>
       </c>
       <c r="Q271" s="108">
-        <f t="shared" ref="Q271:BW271" si="72">1/Q257</f>
+        <f t="shared" ref="Q271:BI271" si="72">1/Q257</f>
         <v>0.18771952200143197</v>
       </c>
       <c r="R271" s="108">
@@ -40182,7 +40182,7 @@
       </c>
       <c r="DR271" s="109"/>
     </row>
-    <row r="272" spans="1:122" s="108" customFormat="1">
+    <row r="272" spans="1:122" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A272" s="108" t="s">
         <v>18</v>
       </c>
@@ -40428,7 +40428,7 @@
       </c>
       <c r="DR272" s="109"/>
     </row>
-    <row r="273" spans="1:122" s="108" customFormat="1">
+    <row r="273" spans="1:122" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A273" s="108" t="s">
         <v>134</v>
       </c>
@@ -40674,16 +40674,16 @@
       </c>
       <c r="DR273" s="109"/>
     </row>
-    <row r="274" spans="1:122" s="108" customFormat="1">
+    <row r="274" spans="1:122" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="DR274" s="109"/>
     </row>
-    <row r="275" spans="1:122" s="108" customFormat="1">
+    <row r="275" spans="1:122" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A275" s="110" t="s">
         <v>151</v>
       </c>
       <c r="DR275" s="109"/>
     </row>
-    <row r="276" spans="1:122" s="111" customFormat="1">
+    <row r="276" spans="1:122" s="111" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A276" s="111" t="s">
         <v>8</v>
       </c>
@@ -40929,7 +40929,7 @@
       </c>
       <c r="DR276" s="112"/>
     </row>
-    <row r="277" spans="1:122" s="111" customFormat="1">
+    <row r="277" spans="1:122" s="111" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A277" s="111" t="s">
         <v>56</v>
       </c>
@@ -41175,7 +41175,7 @@
       </c>
       <c r="DR277" s="112"/>
     </row>
-    <row r="278" spans="1:122" s="111" customFormat="1">
+    <row r="278" spans="1:122" s="111" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A278" s="111" t="s">
         <v>10</v>
       </c>
@@ -41421,7 +41421,7 @@
       </c>
       <c r="DR278" s="112"/>
     </row>
-    <row r="279" spans="1:122" s="111" customFormat="1">
+    <row r="279" spans="1:122" s="111" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A279" s="111" t="s">
         <v>11</v>
       </c>
@@ -41667,7 +41667,7 @@
       </c>
       <c r="DR279" s="112"/>
     </row>
-    <row r="280" spans="1:122" s="111" customFormat="1">
+    <row r="280" spans="1:122" s="111" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A280" s="111" t="s">
         <v>42</v>
       </c>
@@ -41913,7 +41913,7 @@
       </c>
       <c r="DR280" s="112"/>
     </row>
-    <row r="281" spans="1:122" s="111" customFormat="1">
+    <row r="281" spans="1:122" s="111" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A281" s="111" t="s">
         <v>13</v>
       </c>
@@ -42159,7 +42159,7 @@
       </c>
       <c r="DR281" s="112"/>
     </row>
-    <row r="282" spans="1:122" s="111" customFormat="1">
+    <row r="282" spans="1:122" s="111" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A282" s="111" t="s">
         <v>14</v>
       </c>
@@ -42405,7 +42405,7 @@
       </c>
       <c r="DR282" s="112"/>
     </row>
-    <row r="283" spans="1:122" s="111" customFormat="1">
+    <row r="283" spans="1:122" s="111" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A283" s="111" t="s">
         <v>15</v>
       </c>
@@ -42651,7 +42651,7 @@
       </c>
       <c r="DR283" s="112"/>
     </row>
-    <row r="284" spans="1:122" s="111" customFormat="1">
+    <row r="284" spans="1:122" s="111" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A284" s="111" t="s">
         <v>16</v>
       </c>
@@ -42897,7 +42897,7 @@
       </c>
       <c r="DR284" s="112"/>
     </row>
-    <row r="285" spans="1:122" s="111" customFormat="1">
+    <row r="285" spans="1:122" s="111" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A285" s="111" t="s">
         <v>17</v>
       </c>
@@ -43143,7 +43143,7 @@
       </c>
       <c r="DR285" s="112"/>
     </row>
-    <row r="286" spans="1:122" s="111" customFormat="1">
+    <row r="286" spans="1:122" s="111" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A286" s="111" t="s">
         <v>18</v>
       </c>
@@ -43389,7 +43389,7 @@
       </c>
       <c r="DR286" s="112"/>
     </row>
-    <row r="287" spans="1:122" s="111" customFormat="1">
+    <row r="287" spans="1:122" s="111" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A287" s="111" t="s">
         <v>134</v>
       </c>
@@ -43635,7 +43635,7 @@
       </c>
       <c r="DR287" s="112"/>
     </row>
-    <row r="288" spans="1:122" s="108" customFormat="1">
+    <row r="288" spans="1:122" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B288" s="108">
         <f>SUM(B276:B287)</f>
         <v>97.350926624833491</v>
@@ -43878,13 +43878,13 @@
       </c>
       <c r="DR288" s="109"/>
     </row>
-    <row r="289" spans="1:122" s="108" customFormat="1">
+    <row r="289" spans="1:122" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A289" s="110" t="s">
         <v>152</v>
       </c>
       <c r="DR289" s="109"/>
     </row>
-    <row r="290" spans="1:122" s="108" customFormat="1">
+    <row r="290" spans="1:122" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A290" s="108" t="s">
         <v>8</v>
       </c>
@@ -44130,7 +44130,7 @@
       </c>
       <c r="DR290" s="109"/>
     </row>
-    <row r="291" spans="1:122" s="108" customFormat="1">
+    <row r="291" spans="1:122" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A291" s="108" t="s">
         <v>56</v>
       </c>
@@ -44376,7 +44376,7 @@
       </c>
       <c r="DR291" s="109"/>
     </row>
-    <row r="292" spans="1:122" s="108" customFormat="1">
+    <row r="292" spans="1:122" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A292" s="108" t="s">
         <v>10</v>
       </c>
@@ -44622,7 +44622,7 @@
       </c>
       <c r="DR292" s="109"/>
     </row>
-    <row r="293" spans="1:122" s="108" customFormat="1">
+    <row r="293" spans="1:122" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A293" s="108" t="s">
         <v>11</v>
       </c>
@@ -44868,7 +44868,7 @@
       </c>
       <c r="DR293" s="109"/>
     </row>
-    <row r="294" spans="1:122" s="108" customFormat="1">
+    <row r="294" spans="1:122" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A294" s="108" t="s">
         <v>42</v>
       </c>
@@ -45114,7 +45114,7 @@
       </c>
       <c r="DR294" s="109"/>
     </row>
-    <row r="295" spans="1:122" s="108" customFormat="1">
+    <row r="295" spans="1:122" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A295" s="108" t="s">
         <v>13</v>
       </c>
@@ -45179,7 +45179,7 @@
         <v>0.12878130865675586</v>
       </c>
       <c r="Q295" s="108">
-        <f t="shared" ref="Q295:BX295" si="77">+Q281/Q$288</f>
+        <f t="shared" ref="Q295:BI295" si="77">+Q281/Q$288</f>
         <v>0.12881075543009574</v>
       </c>
       <c r="R295" s="108">
@@ -45360,7 +45360,7 @@
       </c>
       <c r="DR295" s="109"/>
     </row>
-    <row r="296" spans="1:122" s="108" customFormat="1">
+    <row r="296" spans="1:122" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A296" s="108" t="s">
         <v>14</v>
       </c>
@@ -45606,7 +45606,7 @@
       </c>
       <c r="DR296" s="109"/>
     </row>
-    <row r="297" spans="1:122" s="108" customFormat="1">
+    <row r="297" spans="1:122" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A297" s="108" t="s">
         <v>15</v>
       </c>
@@ -45852,7 +45852,7 @@
       </c>
       <c r="DR297" s="109"/>
     </row>
-    <row r="298" spans="1:122" s="108" customFormat="1">
+    <row r="298" spans="1:122" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A298" s="108" t="s">
         <v>16</v>
       </c>
@@ -46098,7 +46098,7 @@
       </c>
       <c r="DR298" s="109"/>
     </row>
-    <row r="299" spans="1:122" s="108" customFormat="1">
+    <row r="299" spans="1:122" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A299" s="108" t="s">
         <v>17</v>
       </c>
@@ -46344,7 +46344,7 @@
       </c>
       <c r="DR299" s="109"/>
     </row>
-    <row r="300" spans="1:122" s="108" customFormat="1">
+    <row r="300" spans="1:122" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A300" s="108" t="s">
         <v>18</v>
       </c>
@@ -46409,7 +46409,7 @@
         <v>3.1525726951579819E-2</v>
       </c>
       <c r="Q300" s="108">
-        <f t="shared" ref="Q300:BX300" si="79">+Q286/Q$288</f>
+        <f t="shared" ref="Q300:BI300" si="79">+Q286/Q$288</f>
         <v>3.0943665064492424E-2</v>
       </c>
       <c r="R300" s="108">
@@ -46590,7 +46590,7 @@
       </c>
       <c r="DR300" s="109"/>
     </row>
-    <row r="301" spans="1:122" s="108" customFormat="1">
+    <row r="301" spans="1:122" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A301" s="108" t="s">
         <v>134</v>
       </c>
@@ -46836,7 +46836,7 @@
       </c>
       <c r="DR301" s="109"/>
     </row>
-    <row r="302" spans="1:122" s="108" customFormat="1">
+    <row r="302" spans="1:122" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B302" s="108">
         <f t="shared" ref="B302:I302" si="81">SUM(B290:B301)</f>
         <v>1.0000000000000002</v>
@@ -46871,10 +46871,10 @@
       </c>
       <c r="DR302" s="109"/>
     </row>
-    <row r="303" spans="1:122" s="45" customFormat="1">
+    <row r="303" spans="1:122" s="45" customFormat="1" x14ac:dyDescent="0.2">
       <c r="DR303" s="113"/>
     </row>
-    <row r="304" spans="1:122" s="108" customFormat="1">
+    <row r="304" spans="1:122" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A304" s="110" t="s">
         <v>153</v>
       </c>
@@ -47120,7 +47120,7 @@
       </c>
       <c r="DR304" s="109"/>
     </row>
-    <row r="305" spans="1:122" s="108" customFormat="1">
+    <row r="305" spans="1:122" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A305" s="110" t="s">
         <v>154</v>
       </c>
@@ -47366,7 +47366,7 @@
       </c>
       <c r="DR305" s="109"/>
     </row>
-    <row r="306" spans="1:122" s="108" customFormat="1">
+    <row r="306" spans="1:122" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A306" s="110" t="s">
         <v>155</v>
       </c>
@@ -47612,13 +47612,13 @@
       </c>
       <c r="DR306" s="109"/>
     </row>
-    <row r="307" spans="1:122" s="108" customFormat="1">
+    <row r="307" spans="1:122" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A307" s="110" t="s">
         <v>156</v>
       </c>
       <c r="DR307" s="109"/>
     </row>
-    <row r="308" spans="1:122" s="108" customFormat="1">
+    <row r="308" spans="1:122" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A308" s="110" t="s">
         <v>153</v>
       </c>
@@ -47864,7 +47864,7 @@
       </c>
       <c r="DR308" s="109"/>
     </row>
-    <row r="309" spans="1:122" s="108" customFormat="1">
+    <row r="309" spans="1:122" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A309" s="110" t="s">
         <v>154</v>
       </c>
@@ -48110,7 +48110,7 @@
       </c>
       <c r="DR309" s="109"/>
     </row>
-    <row r="310" spans="1:122" s="108" customFormat="1">
+    <row r="310" spans="1:122" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A310" s="110" t="s">
         <v>155</v>
       </c>
@@ -48356,109 +48356,109 @@
       </c>
       <c r="DR310" s="109"/>
     </row>
-    <row r="311" spans="1:122" s="114" customFormat="1">
+    <row r="311" spans="1:122" s="114" customFormat="1" x14ac:dyDescent="0.2">
       <c r="DR311" s="115"/>
     </row>
-    <row r="312" spans="1:122" s="114" customFormat="1">
+    <row r="312" spans="1:122" s="114" customFormat="1" x14ac:dyDescent="0.2">
       <c r="DR312" s="115"/>
     </row>
-    <row r="313" spans="1:122" s="114" customFormat="1">
+    <row r="313" spans="1:122" s="114" customFormat="1" x14ac:dyDescent="0.2">
       <c r="DR313" s="115"/>
     </row>
-    <row r="314" spans="1:122" s="114" customFormat="1">
+    <row r="314" spans="1:122" s="114" customFormat="1" x14ac:dyDescent="0.2">
       <c r="DR314" s="115"/>
     </row>
-    <row r="315" spans="1:122" s="114" customFormat="1">
+    <row r="315" spans="1:122" s="114" customFormat="1" x14ac:dyDescent="0.2">
       <c r="DR315" s="115"/>
     </row>
-    <row r="316" spans="1:122" s="114" customFormat="1">
+    <row r="316" spans="1:122" s="114" customFormat="1" x14ac:dyDescent="0.2">
       <c r="DR316" s="115"/>
     </row>
-    <row r="317" spans="1:122" s="114" customFormat="1">
+    <row r="317" spans="1:122" s="114" customFormat="1" x14ac:dyDescent="0.2">
       <c r="DR317" s="115"/>
     </row>
-    <row r="318" spans="1:122" s="114" customFormat="1">
+    <row r="318" spans="1:122" s="114" customFormat="1" x14ac:dyDescent="0.2">
       <c r="DR318" s="115"/>
     </row>
-    <row r="319" spans="1:122" s="114" customFormat="1">
+    <row r="319" spans="1:122" s="114" customFormat="1" x14ac:dyDescent="0.2">
       <c r="DR319" s="115"/>
     </row>
-    <row r="320" spans="1:122" s="114" customFormat="1">
+    <row r="320" spans="1:122" s="114" customFormat="1" x14ac:dyDescent="0.2">
       <c r="DR320" s="115"/>
     </row>
-    <row r="321" spans="122:122" s="114" customFormat="1">
+    <row r="321" spans="122:122" s="114" customFormat="1" x14ac:dyDescent="0.2">
       <c r="DR321" s="115"/>
     </row>
-    <row r="322" spans="122:122" s="114" customFormat="1">
+    <row r="322" spans="122:122" s="114" customFormat="1" x14ac:dyDescent="0.2">
       <c r="DR322" s="115"/>
     </row>
-    <row r="323" spans="122:122" s="114" customFormat="1">
+    <row r="323" spans="122:122" s="114" customFormat="1" x14ac:dyDescent="0.2">
       <c r="DR323" s="115"/>
     </row>
-    <row r="324" spans="122:122" s="114" customFormat="1">
+    <row r="324" spans="122:122" s="114" customFormat="1" x14ac:dyDescent="0.2">
       <c r="DR324" s="115"/>
     </row>
-    <row r="325" spans="122:122" s="114" customFormat="1">
+    <row r="325" spans="122:122" s="114" customFormat="1" x14ac:dyDescent="0.2">
       <c r="DR325" s="115"/>
     </row>
-    <row r="326" spans="122:122" s="114" customFormat="1">
+    <row r="326" spans="122:122" s="114" customFormat="1" x14ac:dyDescent="0.2">
       <c r="DR326" s="115"/>
     </row>
-    <row r="327" spans="122:122" s="114" customFormat="1">
+    <row r="327" spans="122:122" s="114" customFormat="1" x14ac:dyDescent="0.2">
       <c r="DR327" s="115"/>
     </row>
-    <row r="328" spans="122:122" s="114" customFormat="1">
+    <row r="328" spans="122:122" s="114" customFormat="1" x14ac:dyDescent="0.2">
       <c r="DR328" s="115"/>
     </row>
-    <row r="329" spans="122:122" s="114" customFormat="1">
+    <row r="329" spans="122:122" s="114" customFormat="1" x14ac:dyDescent="0.2">
       <c r="DR329" s="115"/>
     </row>
-    <row r="330" spans="122:122" s="114" customFormat="1">
+    <row r="330" spans="122:122" s="114" customFormat="1" x14ac:dyDescent="0.2">
       <c r="DR330" s="115"/>
     </row>
-    <row r="331" spans="122:122" s="114" customFormat="1">
+    <row r="331" spans="122:122" s="114" customFormat="1" x14ac:dyDescent="0.2">
       <c r="DR331" s="115"/>
     </row>
-    <row r="332" spans="122:122" s="114" customFormat="1">
+    <row r="332" spans="122:122" s="114" customFormat="1" x14ac:dyDescent="0.2">
       <c r="DR332" s="115"/>
     </row>
-    <row r="333" spans="122:122" s="114" customFormat="1">
+    <row r="333" spans="122:122" s="114" customFormat="1" x14ac:dyDescent="0.2">
       <c r="DR333" s="115"/>
     </row>
-    <row r="334" spans="122:122" s="114" customFormat="1">
+    <row r="334" spans="122:122" s="114" customFormat="1" x14ac:dyDescent="0.2">
       <c r="DR334" s="115"/>
     </row>
-    <row r="335" spans="122:122" s="114" customFormat="1">
+    <row r="335" spans="122:122" s="114" customFormat="1" x14ac:dyDescent="0.2">
       <c r="DR335" s="115"/>
     </row>
-    <row r="336" spans="122:122" s="114" customFormat="1">
+    <row r="336" spans="122:122" s="114" customFormat="1" x14ac:dyDescent="0.2">
       <c r="DR336" s="115"/>
     </row>
-    <row r="337" spans="1:122" s="114" customFormat="1">
+    <row r="337" spans="1:122" s="114" customFormat="1" x14ac:dyDescent="0.2">
       <c r="DR337" s="115"/>
     </row>
-    <row r="338" spans="1:122" s="114" customFormat="1">
+    <row r="338" spans="1:122" s="114" customFormat="1" x14ac:dyDescent="0.2">
       <c r="DR338" s="115"/>
     </row>
-    <row r="339" spans="1:122" s="114" customFormat="1">
+    <row r="339" spans="1:122" s="114" customFormat="1" x14ac:dyDescent="0.2">
       <c r="DR339" s="115"/>
     </row>
-    <row r="340" spans="1:122" s="114" customFormat="1">
+    <row r="340" spans="1:122" s="114" customFormat="1" x14ac:dyDescent="0.2">
       <c r="DR340" s="115"/>
     </row>
-    <row r="341" spans="1:122" s="99" customFormat="1">
+    <row r="341" spans="1:122" s="99" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A341" s="104" t="s">
         <v>157</v>
       </c>
       <c r="DR341" s="100"/>
     </row>
-    <row r="342" spans="1:122" s="99" customFormat="1">
+    <row r="342" spans="1:122" s="99" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A342" s="104" t="s">
         <v>158</v>
       </c>
       <c r="DR342" s="100"/>
     </row>
-    <row r="343" spans="1:122" s="99" customFormat="1">
+    <row r="343" spans="1:122" s="99" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A343" s="104" t="s">
         <v>159</v>
       </c>
@@ -48472,7 +48472,7 @@
       </c>
       <c r="DR343" s="100"/>
     </row>
-    <row r="344" spans="1:122" s="15" customFormat="1">
+    <row r="344" spans="1:122" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A344" s="15" t="s">
         <v>8</v>
       </c>
@@ -48718,7 +48718,7 @@
       </c>
       <c r="DR344" s="116"/>
     </row>
-    <row r="345" spans="1:122" s="15" customFormat="1">
+    <row r="345" spans="1:122" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A345" s="15" t="s">
         <v>56</v>
       </c>
@@ -48964,7 +48964,7 @@
       </c>
       <c r="DR345" s="116"/>
     </row>
-    <row r="346" spans="1:122" s="15" customFormat="1">
+    <row r="346" spans="1:122" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A346" s="15" t="s">
         <v>10</v>
       </c>
@@ -49210,7 +49210,7 @@
       </c>
       <c r="DR346" s="116"/>
     </row>
-    <row r="347" spans="1:122" s="15" customFormat="1">
+    <row r="347" spans="1:122" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A347" s="15" t="s">
         <v>11</v>
       </c>
@@ -49456,7 +49456,7 @@
       </c>
       <c r="DR347" s="116"/>
     </row>
-    <row r="348" spans="1:122" s="15" customFormat="1">
+    <row r="348" spans="1:122" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A348" s="15" t="s">
         <v>42</v>
       </c>
@@ -49521,7 +49521,7 @@
         <v>1.2684891112998049</v>
       </c>
       <c r="Q348" s="15">
-        <f t="shared" ref="Q348:BV348" si="88">+Q252*Q$310</f>
+        <f t="shared" ref="Q348:BI348" si="88">+Q252*Q$310</f>
         <v>1.2856565884788256</v>
       </c>
       <c r="R348" s="15">
@@ -49702,7 +49702,7 @@
       </c>
       <c r="DR348" s="116"/>
     </row>
-    <row r="349" spans="1:122" s="15" customFormat="1">
+    <row r="349" spans="1:122" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A349" s="15" t="s">
         <v>13</v>
       </c>
@@ -49948,7 +49948,7 @@
       </c>
       <c r="DR349" s="116"/>
     </row>
-    <row r="350" spans="1:122" s="15" customFormat="1">
+    <row r="350" spans="1:122" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A350" s="15" t="s">
         <v>14</v>
       </c>
@@ -50194,7 +50194,7 @@
       </c>
       <c r="DR350" s="116"/>
     </row>
-    <row r="351" spans="1:122" s="15" customFormat="1">
+    <row r="351" spans="1:122" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A351" s="15" t="s">
         <v>15</v>
       </c>
@@ -50440,7 +50440,7 @@
       </c>
       <c r="DR351" s="116"/>
     </row>
-    <row r="352" spans="1:122" s="15" customFormat="1">
+    <row r="352" spans="1:122" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A352" s="15" t="s">
         <v>16</v>
       </c>
@@ -50686,7 +50686,7 @@
       </c>
       <c r="DR352" s="116"/>
     </row>
-    <row r="353" spans="1:122" s="15" customFormat="1">
+    <row r="353" spans="1:122" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A353" s="15" t="s">
         <v>17</v>
       </c>
@@ -50751,7 +50751,7 @@
         <v>0.99696950669300621</v>
       </c>
       <c r="Q353" s="15">
-        <f t="shared" ref="Q353:BV353" si="90">+Q257*Q$310</f>
+        <f t="shared" ref="Q353:BI353" si="90">+Q257*Q$310</f>
         <v>0.99596229187486318</v>
       </c>
       <c r="R353" s="15">
@@ -50932,7 +50932,7 @@
       </c>
       <c r="DR353" s="116"/>
     </row>
-    <row r="354" spans="1:122" s="15" customFormat="1">
+    <row r="354" spans="1:122" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A354" s="15" t="s">
         <v>18</v>
       </c>
@@ -51178,7 +51178,7 @@
       </c>
       <c r="DR354" s="116"/>
     </row>
-    <row r="355" spans="1:122" s="15" customFormat="1">
+    <row r="355" spans="1:122" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A355" s="15" t="s">
         <v>134</v>
       </c>
@@ -51424,16 +51424,16 @@
       </c>
       <c r="DR355" s="116"/>
     </row>
-    <row r="356" spans="1:122" s="99" customFormat="1">
+    <row r="356" spans="1:122" s="99" customFormat="1" x14ac:dyDescent="0.2">
       <c r="DR356" s="100"/>
     </row>
-    <row r="357" spans="1:122" s="99" customFormat="1">
+    <row r="357" spans="1:122" s="99" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A357" s="104" t="s">
         <v>160</v>
       </c>
       <c r="DR357" s="100"/>
     </row>
-    <row r="358" spans="1:122" s="99" customFormat="1">
+    <row r="358" spans="1:122" s="99" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A358" s="104" t="s">
         <v>159</v>
       </c>
@@ -51443,7 +51443,7 @@
       </c>
       <c r="DR358" s="100"/>
     </row>
-    <row r="359" spans="1:122" s="117" customFormat="1">
+    <row r="359" spans="1:122" s="117" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A359" s="117" t="s">
         <v>8</v>
       </c>
@@ -51629,7 +51629,7 @@
       </c>
       <c r="DR359" s="118"/>
     </row>
-    <row r="360" spans="1:122" s="117" customFormat="1">
+    <row r="360" spans="1:122" s="117" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A360" s="117" t="s">
         <v>56</v>
       </c>
@@ -51815,7 +51815,7 @@
       </c>
       <c r="DR360" s="118"/>
     </row>
-    <row r="361" spans="1:122" s="117" customFormat="1">
+    <row r="361" spans="1:122" s="117" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A361" s="117" t="s">
         <v>10</v>
       </c>
@@ -52001,7 +52001,7 @@
       </c>
       <c r="DR361" s="118"/>
     </row>
-    <row r="362" spans="1:122" s="117" customFormat="1">
+    <row r="362" spans="1:122" s="117" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A362" s="117" t="s">
         <v>11</v>
       </c>
@@ -52187,7 +52187,7 @@
       </c>
       <c r="DR362" s="118"/>
     </row>
-    <row r="363" spans="1:122" s="117" customFormat="1">
+    <row r="363" spans="1:122" s="117" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A363" s="117" t="s">
         <v>42</v>
       </c>
@@ -52373,7 +52373,7 @@
       </c>
       <c r="DR363" s="118"/>
     </row>
-    <row r="364" spans="1:122" s="117" customFormat="1">
+    <row r="364" spans="1:122" s="117" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A364" s="117" t="s">
         <v>13</v>
       </c>
@@ -52559,7 +52559,7 @@
       </c>
       <c r="DR364" s="118"/>
     </row>
-    <row r="365" spans="1:122" s="117" customFormat="1">
+    <row r="365" spans="1:122" s="117" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A365" s="117" t="s">
         <v>14</v>
       </c>
@@ -52745,7 +52745,7 @@
       </c>
       <c r="DR365" s="118"/>
     </row>
-    <row r="366" spans="1:122" s="117" customFormat="1">
+    <row r="366" spans="1:122" s="117" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A366" s="117" t="s">
         <v>15</v>
       </c>
@@ -52931,7 +52931,7 @@
       </c>
       <c r="DR366" s="118"/>
     </row>
-    <row r="367" spans="1:122" s="117" customFormat="1">
+    <row r="367" spans="1:122" s="117" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A367" s="117" t="s">
         <v>16</v>
       </c>
@@ -53117,7 +53117,7 @@
       </c>
       <c r="DR367" s="118"/>
     </row>
-    <row r="368" spans="1:122" s="117" customFormat="1">
+    <row r="368" spans="1:122" s="117" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A368" s="117" t="s">
         <v>17</v>
       </c>
@@ -53303,7 +53303,7 @@
       </c>
       <c r="DR368" s="118"/>
     </row>
-    <row r="369" spans="1:122" s="117" customFormat="1">
+    <row r="369" spans="1:122" s="117" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A369" s="117" t="s">
         <v>18</v>
       </c>
@@ -53489,7 +53489,7 @@
       </c>
       <c r="DR369" s="118"/>
     </row>
-    <row r="370" spans="1:122" s="117" customFormat="1">
+    <row r="370" spans="1:122" s="117" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A370" s="117" t="s">
         <v>134</v>
       </c>
@@ -53675,7 +53675,7 @@
       </c>
       <c r="DR370" s="118"/>
     </row>
-    <row r="374" spans="1:122" s="43" customFormat="1">
+    <row r="374" spans="1:122" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A374" s="58" t="s">
         <v>161</v>
       </c>
@@ -53804,7 +53804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="375" spans="1:122" s="119" customFormat="1">
+    <row r="375" spans="1:122" s="119" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A375" s="119" t="s">
         <v>8</v>
       </c>
@@ -53899,7 +53899,7 @@
         <v>2.3885051393862582E-4</v>
       </c>
     </row>
-    <row r="376" spans="1:122" s="119" customFormat="1">
+    <row r="376" spans="1:122" s="119" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A376" s="119" t="s">
         <v>9</v>
       </c>
@@ -53994,7 +53994,7 @@
         <v>3.1396723190096556E-4</v>
       </c>
     </row>
-    <row r="377" spans="1:122" s="119" customFormat="1">
+    <row r="377" spans="1:122" s="119" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A377" s="119" t="s">
         <v>10</v>
       </c>
@@ -54089,7 +54089,7 @@
         <v>3.0840332648654197E-4</v>
       </c>
     </row>
-    <row r="378" spans="1:122" s="119" customFormat="1">
+    <row r="378" spans="1:122" s="119" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A378" s="119" t="s">
         <v>11</v>
       </c>
@@ -54184,7 +54184,7 @@
         <v>2.7494542668942047E-4</v>
       </c>
     </row>
-    <row r="379" spans="1:122" s="119" customFormat="1">
+    <row r="379" spans="1:122" s="119" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A379" s="119" t="s">
         <v>12</v>
       </c>
@@ -54279,7 +54279,7 @@
         <v>2.6712831904026366E-4</v>
       </c>
     </row>
-    <row r="380" spans="1:122" s="119" customFormat="1">
+    <row r="380" spans="1:122" s="119" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A380" s="119" t="s">
         <v>13</v>
       </c>
@@ -54374,7 +54374,7 @@
         <v>3.400889125551121E-4</v>
       </c>
     </row>
-    <row r="381" spans="1:122" s="119" customFormat="1">
+    <row r="381" spans="1:122" s="119" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A381" s="119" t="s">
         <v>162</v>
       </c>
@@ -54469,7 +54469,7 @@
         <v>2.510562290461483E-4</v>
       </c>
     </row>
-    <row r="382" spans="1:122" s="119" customFormat="1">
+    <row r="382" spans="1:122" s="119" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A382" s="119" t="s">
         <v>15</v>
       </c>
@@ -54564,7 +54564,7 @@
         <v>2.3184833799830409E-4</v>
       </c>
     </row>
-    <row r="383" spans="1:122" s="119" customFormat="1">
+    <row r="383" spans="1:122" s="119" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A383" s="119" t="s">
         <v>16</v>
       </c>
@@ -54689,7 +54689,7 @@
         <v>-7.463066265336177E-4</v>
       </c>
     </row>
-    <row r="384" spans="1:122" s="119" customFormat="1">
+    <row r="384" spans="1:122" s="119" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A384" s="119" t="s">
         <v>17</v>
       </c>
@@ -54784,7 +54784,7 @@
         <v>2.9863628279880783E-4</v>
       </c>
     </row>
-    <row r="385" spans="1:59" s="119" customFormat="1">
+    <row r="385" spans="1:59" s="119" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A385" s="119" t="s">
         <v>18</v>
       </c>
@@ -54879,7 +54879,7 @@
         <v>3.0167347725146889E-4</v>
       </c>
     </row>
-    <row r="386" spans="1:59" s="119" customFormat="1">
+    <row r="386" spans="1:59" s="119" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A386" s="119" t="s">
         <v>19</v>
       </c>
@@ -54974,7 +54974,7 @@
         <v>2.4588974617446705E-4</v>
       </c>
     </row>
-    <row r="387" spans="1:59" s="43" customFormat="1">
+    <row r="387" spans="1:59" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B387" s="48"/>
       <c r="C387" s="48"/>
       <c r="D387" s="48"/>
@@ -55034,17 +55034,17 @@
       <c r="BF387" s="48"/>
       <c r="BG387" s="48"/>
     </row>
-    <row r="388" spans="1:59" s="43" customFormat="1">
+    <row r="388" spans="1:59" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A388" s="45"/>
     </row>
-    <row r="389" spans="1:59" s="43" customFormat="1">
+    <row r="389" spans="1:59" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A389" s="39"/>
       <c r="B389" s="119">
         <v>9.3279313555020352E-3</v>
       </c>
     </row>
-    <row r="390" spans="1:59" s="43" customFormat="1"/>
-    <row r="391" spans="1:59">
+    <row r="390" spans="1:59" s="43" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="391" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A391" t="s">
         <v>163</v>
       </c>
@@ -55168,7 +55168,7 @@
         <v>-1E-3</v>
       </c>
     </row>
-    <row r="392" spans="1:59" s="119" customFormat="1">
+    <row r="392" spans="1:59" s="119" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A392" s="119" t="s">
         <v>16</v>
       </c>
@@ -55263,7 +55263,7 @@
         <v>2.5369337346638232E-4</v>
       </c>
     </row>
-    <row r="393" spans="1:59">
+    <row r="393" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A393" t="s">
         <v>164</v>
       </c>
@@ -55388,10 +55388,10 @@
         <v>-7.463066265336177E-4</v>
       </c>
     </row>
-    <row r="394" spans="1:59">
+    <row r="394" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A394" s="9"/>
     </row>
-    <row r="395" spans="1:59">
+    <row r="395" spans="1:59" x14ac:dyDescent="0.2">
       <c r="C395" s="16"/>
       <c r="D395" s="16"/>
       <c r="E395" s="16"/>
@@ -55402,12 +55402,12 @@
       <c r="J395" s="16"/>
       <c r="K395" s="16"/>
     </row>
-    <row r="396" spans="1:59">
+    <row r="396" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A396" s="9" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="397" spans="1:59">
+    <row r="397" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A397" t="s">
         <v>166</v>
       </c>
@@ -55531,7 +55531,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="398" spans="1:59">
+    <row r="398" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A398" t="s">
         <v>198</v>
       </c>
@@ -55655,7 +55655,7 @@
         <v>1622101.8434109497</v>
       </c>
     </row>
-    <row r="399" spans="1:59">
+    <row r="399" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A399" t="s">
         <v>198</v>
       </c>
@@ -55779,7 +55779,7 @@
         <v>989662.3730919793</v>
       </c>
     </row>
-    <row r="400" spans="1:59">
+    <row r="400" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A400" t="s">
         <v>198</v>
       </c>
@@ -55903,7 +55903,7 @@
         <v>381874.40790214809</v>
       </c>
     </row>
-    <row r="401" spans="1:62">
+    <row r="401" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A401" t="s">
         <v>198</v>
       </c>
@@ -56027,7 +56027,7 @@
         <v>422812.10034219554</v>
       </c>
     </row>
-    <row r="402" spans="1:62">
+    <row r="402" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A402" t="s">
         <v>198</v>
       </c>
@@ -56151,7 +56151,7 @@
         <v>233303.761067168</v>
       </c>
     </row>
-    <row r="403" spans="1:62">
+    <row r="403" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A403" t="s">
         <v>198</v>
       </c>
@@ -56275,7 +56275,7 @@
         <v>2842414.0207481277</v>
       </c>
     </row>
-    <row r="404" spans="1:62">
+    <row r="404" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A404" t="s">
         <v>198</v>
       </c>
@@ -56399,7 +56399,7 @@
         <v>722982.07324102172</v>
       </c>
     </row>
-    <row r="405" spans="1:62">
+    <row r="405" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A405" t="s">
         <v>198</v>
       </c>
@@ -56523,7 +56523,7 @@
         <v>806274.90940003714</v>
       </c>
     </row>
-    <row r="406" spans="1:62">
+    <row r="406" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A406" t="s">
         <v>198</v>
       </c>
@@ -56647,7 +56647,7 @@
         <v>243782.86421170569</v>
       </c>
     </row>
-    <row r="407" spans="1:62">
+    <row r="407" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A407" t="s">
         <v>198</v>
       </c>
@@ -56771,7 +56771,7 @@
         <v>532456.37372195767</v>
       </c>
     </row>
-    <row r="408" spans="1:62">
+    <row r="408" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A408" t="s">
         <v>198</v>
       </c>
@@ -56895,7 +56895,7 @@
         <v>568855.94567984424</v>
       </c>
     </row>
-    <row r="409" spans="1:62">
+    <row r="409" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A409" s="9" t="s">
         <v>198</v>
       </c>
@@ -57019,7 +57019,7 @@
         <v>630876.96868782956</v>
       </c>
     </row>
-    <row r="410" spans="1:62">
+    <row r="410" spans="1:62" x14ac:dyDescent="0.2">
       <c r="G410">
         <v>5332000.0000000019</v>
       </c>
@@ -57129,7 +57129,7 @@
         <v>9997397.641504962</v>
       </c>
     </row>
-    <row r="411" spans="1:62" s="123" customFormat="1" ht="18" customHeight="1">
+    <row r="411" spans="1:62" s="123" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A411" s="121"/>
       <c r="B411" s="122">
         <v>2005</v>
@@ -57375,12 +57375,12 @@
         <v>2605</v>
       </c>
     </row>
-    <row r="412" spans="1:62" ht="21.75" customHeight="1">
+    <row r="412" spans="1:62" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A412" s="23" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="413" spans="1:62" s="30" customFormat="1">
+    <row r="413" spans="1:62" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A413" t="s">
         <v>8</v>
       </c>
@@ -57473,7 +57473,7 @@
         <v>2.6394667696416914</v>
       </c>
     </row>
-    <row r="414" spans="1:62" s="30" customFormat="1">
+    <row r="414" spans="1:62" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A414" s="9" t="s">
         <v>56</v>
       </c>
@@ -57566,7 +57566,7 @@
         <v>1.8592463887239199</v>
       </c>
     </row>
-    <row r="415" spans="1:62" s="30" customFormat="1">
+    <row r="415" spans="1:62" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A415" t="s">
         <v>10</v>
       </c>
@@ -57659,7 +57659,7 @@
         <v>0.37138821559282664</v>
       </c>
     </row>
-    <row r="416" spans="1:62" s="30" customFormat="1">
+    <row r="416" spans="1:62" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A416" t="s">
         <v>11</v>
       </c>
@@ -57752,7 +57752,7 @@
         <v>0.6322762867738172</v>
       </c>
     </row>
-    <row r="417" spans="1:23" s="30" customFormat="1">
+    <row r="417" spans="1:23" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A417" t="s">
         <v>42</v>
       </c>
@@ -57845,7 +57845,7 @@
         <v>0.4932274806331064</v>
       </c>
     </row>
-    <row r="418" spans="1:23" s="30" customFormat="1">
+    <row r="418" spans="1:23" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A418" t="s">
         <v>13</v>
       </c>
@@ -57938,7 +57938,7 @@
         <v>4.5744276190461139</v>
       </c>
     </row>
-    <row r="419" spans="1:23" s="30" customFormat="1">
+    <row r="419" spans="1:23" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A419" t="s">
         <v>14</v>
       </c>
@@ -58031,7 +58031,7 @@
         <v>3.3647211053071073</v>
       </c>
     </row>
-    <row r="420" spans="1:23" s="30" customFormat="1">
+    <row r="420" spans="1:23" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A420" t="s">
         <v>15</v>
       </c>
@@ -58124,7 +58124,7 @@
         <v>3.0053335151292324</v>
       </c>
     </row>
-    <row r="421" spans="1:23" s="30" customFormat="1">
+    <row r="421" spans="1:23" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A421" t="s">
         <v>16</v>
       </c>
@@ -58217,7 +58217,7 @@
         <v>1.8634157086655028</v>
       </c>
     </row>
-    <row r="422" spans="1:23" s="30" customFormat="1">
+    <row r="422" spans="1:23" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A422" t="s">
         <v>17</v>
       </c>
@@ -58310,7 +58310,7 @@
         <v>2.140673514253578</v>
       </c>
     </row>
-    <row r="423" spans="1:23" s="30" customFormat="1">
+    <row r="423" spans="1:23" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A423" t="s">
         <v>18</v>
       </c>
@@ -58403,7 +58403,7 @@
         <v>0.7144341493965134</v>
       </c>
     </row>
-    <row r="424" spans="1:23" s="30" customFormat="1">
+    <row r="424" spans="1:23" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A424" t="s">
         <v>19</v>
       </c>
@@ -58496,7 +58496,7 @@
         <v>4.8917808064143493</v>
       </c>
     </row>
-    <row r="425" spans="1:23" s="30" customFormat="1">
+    <row r="425" spans="1:23" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B425" s="30">
         <f>SUM(B413:B424)</f>
         <v>7.9676363556275431</v>
@@ -58586,10 +58586,10 @@
         <v>26.550391559577761</v>
       </c>
     </row>
-    <row r="426" spans="1:23">
+    <row r="426" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A426" s="9"/>
     </row>
-    <row r="427" spans="1:23">
+    <row r="427" spans="1:23" ht="16" x14ac:dyDescent="0.25">
       <c r="A427" s="125"/>
       <c r="E427" s="125"/>
       <c r="F427" s="125"/>
@@ -58599,16 +58599,16 @@
       <c r="J427" s="125"/>
       <c r="K427" s="125"/>
     </row>
-    <row r="428" spans="1:23">
+    <row r="428" spans="1:23" x14ac:dyDescent="0.2">
       <c r="J428" s="7"/>
     </row>
-    <row r="429" spans="1:23">
+    <row r="429" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A429" s="9"/>
     </row>
-    <row r="433" spans="1:13">
+    <row r="433" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A433" s="9"/>
     </row>
-    <row r="434" spans="1:13">
+    <row r="434" spans="1:13" ht="16" x14ac:dyDescent="0.25">
       <c r="A434" s="125"/>
       <c r="E434" s="125"/>
       <c r="F434" s="125"/>
@@ -58618,64 +58618,64 @@
       <c r="J434" s="125"/>
       <c r="K434" s="125"/>
     </row>
-    <row r="435" spans="1:13" s="16" customFormat="1"/>
-    <row r="436" spans="1:13" s="16" customFormat="1">
+    <row r="435" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="436" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J436"/>
       <c r="K436"/>
     </row>
-    <row r="437" spans="1:13" s="16" customFormat="1"/>
-    <row r="438" spans="1:13" s="16" customFormat="1"/>
-    <row r="439" spans="1:13" s="16" customFormat="1"/>
-    <row r="440" spans="1:13" s="16" customFormat="1"/>
-    <row r="441" spans="1:13" s="16" customFormat="1">
+    <row r="437" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="438" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="439" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="440" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="441" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A441" s="9"/>
     </row>
-    <row r="442" spans="1:13" s="16" customFormat="1">
+    <row r="442" spans="1:13" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.25">
       <c r="A442"/>
       <c r="J442" s="126"/>
       <c r="K442" s="126"/>
     </row>
-    <row r="443" spans="1:13" s="16" customFormat="1">
+    <row r="443" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A443" s="9"/>
     </row>
-    <row r="444" spans="1:13" s="16" customFormat="1">
+    <row r="444" spans="1:13" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.25">
       <c r="A444"/>
       <c r="M444" s="126"/>
     </row>
-    <row r="445" spans="1:13" s="16" customFormat="1">
+    <row r="445" spans="1:13" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.25">
       <c r="A445"/>
       <c r="M445" s="126"/>
     </row>
-    <row r="446" spans="1:13" s="16" customFormat="1">
+    <row r="446" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A446"/>
     </row>
-    <row r="447" spans="1:13" s="16" customFormat="1">
+    <row r="447" spans="1:13" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.25">
       <c r="A447"/>
       <c r="J447" s="126"/>
       <c r="K447" s="126"/>
     </row>
-    <row r="448" spans="1:13" s="16" customFormat="1">
+    <row r="448" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A448"/>
     </row>
-    <row r="449" spans="1:1" s="16" customFormat="1">
+    <row r="449" spans="1:1" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A449"/>
     </row>
-    <row r="450" spans="1:1" s="16" customFormat="1">
+    <row r="450" spans="1:1" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A450"/>
     </row>
-    <row r="451" spans="1:1" s="16" customFormat="1">
+    <row r="451" spans="1:1" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A451"/>
     </row>
-    <row r="452" spans="1:1" s="16" customFormat="1">
+    <row r="452" spans="1:1" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A452"/>
     </row>
-    <row r="453" spans="1:1" s="16" customFormat="1">
+    <row r="453" spans="1:1" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A453"/>
     </row>
-    <row r="454" spans="1:1" s="16" customFormat="1">
+    <row r="454" spans="1:1" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A454" s="9"/>
     </row>
-    <row r="455" spans="1:1" s="16" customFormat="1"/>
+    <row r="455" spans="1:1" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>